<commit_message>
Starting to work with it
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{721773D7-A6A1-4A56-8FF1-AE9ED364AB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B2490B-1AC4-43F8-BA46-1DA9B0CE4E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Day</t>
   </si>
@@ -93,6 +93,78 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Absicht haben</t>
+  </si>
+  <si>
+    <t>to have the intention</t>
+  </si>
+  <si>
+    <t>Angst haben</t>
+  </si>
+  <si>
+    <t>to be afraid</t>
+  </si>
+  <si>
+    <t>einen Vogel haben</t>
+  </si>
+  <si>
+    <t>Erfolg haben</t>
+  </si>
+  <si>
+    <t>to be successful</t>
+  </si>
+  <si>
+    <t>Glück haben</t>
+  </si>
+  <si>
+    <t>to be lucky</t>
+  </si>
+  <si>
+    <t>Hunger haben</t>
+  </si>
+  <si>
+    <t>to be hungry</t>
+  </si>
+  <si>
+    <t>im Auge haben</t>
+  </si>
+  <si>
+    <t>to have in mind</t>
+  </si>
+  <si>
+    <t>im Griff haben</t>
+  </si>
+  <si>
+    <t>to have under control</t>
+  </si>
+  <si>
+    <t>Pech haben</t>
+  </si>
+  <si>
+    <t>to be unlucky</t>
+  </si>
+  <si>
+    <t>Probleme haben</t>
+  </si>
+  <si>
+    <t>to have problems</t>
+  </si>
+  <si>
+    <t>recht haben</t>
+  </si>
+  <si>
+    <t>to be right</t>
+  </si>
+  <si>
+    <t>to be crazy (literally to have a bird)</t>
+  </si>
+  <si>
+    <t>German Stub</t>
+  </si>
+  <si>
+    <t>English Stub</t>
   </si>
 </sst>
 </file>
@@ -1115,15 +1187,45 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="10">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{CF0BFCF7-580A-46F8-B3AF-2ED41BABC61B}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB114D2F-F620-446A-92CE-0CB3C9FD0F74}">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A8:P40"/>
+  <dimension ref="A7:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1131,10 +1233,13 @@
     <col min="3" max="5" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.33203125" customWidth="1"/>
     <col min="7" max="10" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.109375" customWidth="1"/>
+    <col min="16" max="16" width="39.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:16" ht="103.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:16" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:16" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1169,8 +1274,6 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" cm="1">
@@ -1185,8 +1288,14 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>2</v>
       </c>
@@ -1198,6 +1307,12 @@
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="10"/>
+      <c r="O11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
@@ -1211,6 +1326,12 @@
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="10"/>
+      <c r="O12" t="s">
+        <v>13</v>
+      </c>
+      <c r="P12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
@@ -1224,6 +1345,12 @@
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="10"/>
+      <c r="O13" t="s">
+        <v>15</v>
+      </c>
+      <c r="P13" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
@@ -1237,6 +1364,12 @@
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="10"/>
+      <c r="O14" t="s">
+        <v>16</v>
+      </c>
+      <c r="P14" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
@@ -1250,6 +1383,12 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="10"/>
+      <c r="O15" t="s">
+        <v>18</v>
+      </c>
+      <c r="P15" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
@@ -1263,8 +1402,14 @@
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="10"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>20</v>
+      </c>
+      <c r="P16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>8</v>
       </c>
@@ -1276,8 +1421,14 @@
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="10"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>22</v>
+      </c>
+      <c r="P17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <v>9</v>
       </c>
@@ -1289,8 +1440,14 @@
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="10"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>24</v>
+      </c>
+      <c r="P18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>10</v>
       </c>
@@ -1302,8 +1459,14 @@
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="10"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="O19" t="s">
+        <v>26</v>
+      </c>
+      <c r="P19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="5">
         <v>11</v>
       </c>
@@ -1315,8 +1478,14 @@
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="10"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="O20" t="s">
+        <v>28</v>
+      </c>
+      <c r="P20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="5">
         <v>12</v>
       </c>
@@ -1340,21 +1509,35 @@
         <v>10</v>
       </c>
       <c r="J21" s="10"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="O21" t="s">
+        <v>30</v>
+      </c>
+      <c r="P21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="5">
         <v>13</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
+      <c r="C22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
+      <c r="G22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="I22" s="9"/>
       <c r="J22" s="10"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
         <v>14</v>
       </c>
@@ -1367,7 +1550,7 @@
       <c r="I23" s="9"/>
       <c r="J23" s="10"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="5">
         <v>15</v>
       </c>
@@ -1380,7 +1563,7 @@
       <c r="I24" s="9"/>
       <c r="J24" s="10"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
         <v>16</v>
       </c>
@@ -1393,7 +1576,7 @@
       <c r="I25" s="9"/>
       <c r="J25" s="10"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
         <v>17</v>
       </c>
@@ -1406,7 +1589,7 @@
       <c r="I26" s="9"/>
       <c r="J26" s="10"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
         <v>18</v>
       </c>
@@ -1419,7 +1602,7 @@
       <c r="I27" s="9"/>
       <c r="J27" s="10"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
         <v>19</v>
       </c>
@@ -1432,7 +1615,7 @@
       <c r="I28" s="9"/>
       <c r="J28" s="10"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="5">
         <v>20</v>
       </c>
@@ -1445,7 +1628,7 @@
       <c r="I29" s="9"/>
       <c r="J29" s="10"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="5">
         <v>21</v>
       </c>
@@ -1458,7 +1641,7 @@
       <c r="I30" s="9"/>
       <c r="J30" s="10"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="5">
         <v>22</v>
       </c>
@@ -1471,7 +1654,7 @@
       <c r="I31" s="9"/>
       <c r="J31" s="10"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="5">
         <v>23</v>
       </c>
@@ -1589,6 +1772,9 @@
       <c r="J40" s="13"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O16:O36">
+    <sortCondition ref="O16:O36"/>
+  </sortState>
   <conditionalFormatting sqref="B10:J40">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(B10)-ROW($B$9),2)</formula>

</xml_diff>

<commit_message>
Today's daily planner with simple past drill
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A4721E-208E-4365-8770-B398B2159537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AF7FFF-B793-49BC-BA63-B0D9A0A1F3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$Q$24:$Q$60</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$B$9:$L$40</definedName>
   </definedNames>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="94">
   <si>
     <t>Day</t>
   </si>
@@ -171,6 +172,177 @@
   </si>
   <si>
     <t>Stat Drill</t>
+  </si>
+  <si>
+    <t>sein (to be) - war</t>
+  </si>
+  <si>
+    <t>haben (to have) - hatte</t>
+  </si>
+  <si>
+    <t>werden (to become) - wurde</t>
+  </si>
+  <si>
+    <t>können (can) - konnte</t>
+  </si>
+  <si>
+    <t>müssen (must) - musste</t>
+  </si>
+  <si>
+    <t>sagen (to say) - sagte</t>
+  </si>
+  <si>
+    <t>machen (to make/do) - machte</t>
+  </si>
+  <si>
+    <t>geben (to give) - gab</t>
+  </si>
+  <si>
+    <t>kommen (to come) - kam</t>
+  </si>
+  <si>
+    <t>sollen (should) - sollte</t>
+  </si>
+  <si>
+    <t>wollen (to want) - wollte</t>
+  </si>
+  <si>
+    <t>gehen (to go) - ging</t>
+  </si>
+  <si>
+    <t>wissen (to know) - wusste</t>
+  </si>
+  <si>
+    <t>sehen (to see) - sah</t>
+  </si>
+  <si>
+    <t>lassen (to let/allow) - ließ</t>
+  </si>
+  <si>
+    <t>stehen (to stand) - stand</t>
+  </si>
+  <si>
+    <t>finden (to find) - fand</t>
+  </si>
+  <si>
+    <t>bleiben (to stay) - blieb</t>
+  </si>
+  <si>
+    <t>liegen (to lie) - lag</t>
+  </si>
+  <si>
+    <t>sein (to be)</t>
+  </si>
+  <si>
+    <t>war</t>
+  </si>
+  <si>
+    <t>bleiben (to stay)</t>
+  </si>
+  <si>
+    <t>blieb</t>
+  </si>
+  <si>
+    <t>finden (to find)</t>
+  </si>
+  <si>
+    <t>fand</t>
+  </si>
+  <si>
+    <t>geben (to give)</t>
+  </si>
+  <si>
+    <t>gab</t>
+  </si>
+  <si>
+    <t>gehen (to go)</t>
+  </si>
+  <si>
+    <t>ging</t>
+  </si>
+  <si>
+    <t>haben (to have)</t>
+  </si>
+  <si>
+    <t>hatte</t>
+  </si>
+  <si>
+    <t>kommen (to come)</t>
+  </si>
+  <si>
+    <t>kam</t>
+  </si>
+  <si>
+    <t>können (can)</t>
+  </si>
+  <si>
+    <t>konnte</t>
+  </si>
+  <si>
+    <t>lassen (to let/allow)</t>
+  </si>
+  <si>
+    <t>ließ</t>
+  </si>
+  <si>
+    <t>liegen (to lie)</t>
+  </si>
+  <si>
+    <t>lag</t>
+  </si>
+  <si>
+    <t>machen (to make/do)</t>
+  </si>
+  <si>
+    <t>machte</t>
+  </si>
+  <si>
+    <t>müssen (must)</t>
+  </si>
+  <si>
+    <t>musste</t>
+  </si>
+  <si>
+    <t>sagen (to say)</t>
+  </si>
+  <si>
+    <t>sagte</t>
+  </si>
+  <si>
+    <t>sehen (to see)</t>
+  </si>
+  <si>
+    <t>sah</t>
+  </si>
+  <si>
+    <t>sollen (should)</t>
+  </si>
+  <si>
+    <t>sollte</t>
+  </si>
+  <si>
+    <t>stehen (to stand)</t>
+  </si>
+  <si>
+    <t>stand</t>
+  </si>
+  <si>
+    <t>werden (to become)</t>
+  </si>
+  <si>
+    <t>wurde</t>
+  </si>
+  <si>
+    <t>wissen (to know)</t>
+  </si>
+  <si>
+    <t>wusste</t>
+  </si>
+  <si>
+    <t>wollen (to want)</t>
+  </si>
+  <si>
+    <t>wollte</t>
   </si>
 </sst>
 </file>
@@ -1270,10 +1442,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A7:R40"/>
+  <dimension ref="A7:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24:S42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1479,7 +1651,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>8</v>
       </c>
@@ -1500,7 +1672,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <v>9</v>
       </c>
@@ -1521,7 +1693,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>10</v>
       </c>
@@ -1542,7 +1714,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20" s="5">
         <v>11</v>
       </c>
@@ -1563,7 +1735,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="5">
         <v>12</v>
       </c>
@@ -1598,7 +1770,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="5">
         <v>13</v>
       </c>
@@ -1629,22 +1801,38 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
         <v>14</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="15"/>
+      <c r="C23" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>9</v>
+      </c>
       <c r="K23" s="15"/>
       <c r="L23" s="10"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24" s="5">
         <v>15</v>
       </c>
@@ -1658,8 +1846,17 @@
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
       <c r="L24" s="10"/>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q24" t="s">
+        <v>37</v>
+      </c>
+      <c r="R24" t="s">
+        <v>56</v>
+      </c>
+      <c r="S24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
         <v>16</v>
       </c>
@@ -1673,8 +1870,17 @@
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
       <c r="L25" s="10"/>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q25" t="s">
+        <v>54</v>
+      </c>
+      <c r="R25" t="s">
+        <v>58</v>
+      </c>
+      <c r="S25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
         <v>17</v>
       </c>
@@ -1688,8 +1894,17 @@
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
       <c r="L26" s="10"/>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q26" t="s">
+        <v>53</v>
+      </c>
+      <c r="R26" t="s">
+        <v>60</v>
+      </c>
+      <c r="S26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
         <v>18</v>
       </c>
@@ -1703,8 +1918,17 @@
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
       <c r="L27" s="10"/>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q27" t="s">
+        <v>44</v>
+      </c>
+      <c r="R27" t="s">
+        <v>62</v>
+      </c>
+      <c r="S27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
         <v>19</v>
       </c>
@@ -1718,8 +1942,17 @@
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
       <c r="L28" s="10"/>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q28" t="s">
+        <v>48</v>
+      </c>
+      <c r="R28" t="s">
+        <v>64</v>
+      </c>
+      <c r="S28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B29" s="5">
         <v>20</v>
       </c>
@@ -1733,8 +1966,17 @@
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
       <c r="L29" s="10"/>
-    </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q29" t="s">
+        <v>38</v>
+      </c>
+      <c r="R29" t="s">
+        <v>66</v>
+      </c>
+      <c r="S29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B30" s="5">
         <v>21</v>
       </c>
@@ -1748,8 +1990,17 @@
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
       <c r="L30" s="10"/>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q30" t="s">
+        <v>45</v>
+      </c>
+      <c r="R30" t="s">
+        <v>68</v>
+      </c>
+      <c r="S30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B31" s="5">
         <v>22</v>
       </c>
@@ -1763,8 +2014,17 @@
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
       <c r="L31" s="10"/>
-    </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q31" t="s">
+        <v>40</v>
+      </c>
+      <c r="R31" t="s">
+        <v>70</v>
+      </c>
+      <c r="S31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B32" s="5">
         <v>23</v>
       </c>
@@ -1778,8 +2038,17 @@
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
       <c r="L32" s="10"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="Q32" t="s">
+        <v>51</v>
+      </c>
+      <c r="R32" t="s">
+        <v>72</v>
+      </c>
+      <c r="S32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B33" s="5">
         <v>24</v>
       </c>
@@ -1793,8 +2062,17 @@
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
       <c r="L33" s="10"/>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="Q33" t="s">
+        <v>55</v>
+      </c>
+      <c r="R33" t="s">
+        <v>74</v>
+      </c>
+      <c r="S33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B34" s="5">
         <v>25</v>
       </c>
@@ -1808,8 +2086,17 @@
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
       <c r="L34" s="10"/>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="Q34" t="s">
+        <v>43</v>
+      </c>
+      <c r="R34" t="s">
+        <v>76</v>
+      </c>
+      <c r="S34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B35" s="5">
         <v>26</v>
       </c>
@@ -1823,8 +2110,17 @@
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
       <c r="L35" s="10"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="Q35" t="s">
+        <v>41</v>
+      </c>
+      <c r="R35" t="s">
+        <v>78</v>
+      </c>
+      <c r="S35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B36" s="5">
         <v>27</v>
       </c>
@@ -1838,8 +2134,17 @@
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
       <c r="L36" s="10"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="Q36" t="s">
+        <v>42</v>
+      </c>
+      <c r="R36" t="s">
+        <v>80</v>
+      </c>
+      <c r="S36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B37" s="5">
         <v>28</v>
       </c>
@@ -1853,8 +2158,17 @@
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
       <c r="L37" s="10"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="Q37" t="s">
+        <v>50</v>
+      </c>
+      <c r="R37" t="s">
+        <v>82</v>
+      </c>
+      <c r="S37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B38" s="5">
         <v>29</v>
       </c>
@@ -1868,8 +2182,17 @@
       <c r="J38" s="15"/>
       <c r="K38" s="15"/>
       <c r="L38" s="10"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="Q38" t="s">
+        <v>46</v>
+      </c>
+      <c r="R38" t="s">
+        <v>84</v>
+      </c>
+      <c r="S38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B39" s="5">
         <v>30</v>
       </c>
@@ -1883,8 +2206,17 @@
       <c r="J39" s="15"/>
       <c r="K39" s="15"/>
       <c r="L39" s="10"/>
-    </row>
-    <row r="40" spans="2:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q39" t="s">
+        <v>52</v>
+      </c>
+      <c r="R39" t="s">
+        <v>86</v>
+      </c>
+      <c r="S39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="6">
         <v>31</v>
       </c>
@@ -1898,6 +2230,37 @@
       <c r="J40" s="16"/>
       <c r="K40" s="16"/>
       <c r="L40" s="13"/>
+      <c r="Q40" t="s">
+        <v>39</v>
+      </c>
+      <c r="R40" t="s">
+        <v>88</v>
+      </c>
+      <c r="S40" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Q41" t="s">
+        <v>49</v>
+      </c>
+      <c r="R41" t="s">
+        <v>90</v>
+      </c>
+      <c r="S41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Q42" t="s">
+        <v>47</v>
+      </c>
+      <c r="R42" t="s">
+        <v>92</v>
+      </c>
+      <c r="S42" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Q16:Q36">

</xml_diff>

<commit_message>
Met minimum for today
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D68F6FA-9613-44EC-AD3D-751F83DFB634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C662C3-85DC-459E-9AED-69E8A52BC76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$Q$24:$Q$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$R$24:$R$60</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$B$9:$L$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$B$9:$M$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="96">
   <si>
     <t>Day</t>
   </si>
@@ -343,6 +343,12 @@
   </si>
   <si>
     <t>knew</t>
+  </si>
+  <si>
+    <t>Emoji List</t>
+  </si>
+  <si>
+    <t>Excel Drill</t>
   </si>
 </sst>
 </file>
@@ -1442,27 +1448,29 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A7:S42"/>
+  <dimension ref="A7:W80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="5" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.33203125" customWidth="1"/>
-    <col min="7" max="9" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="3.33203125" customWidth="1"/>
-    <col min="12" max="12" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.109375" customWidth="1"/>
-    <col min="18" max="18" width="24.5546875" customWidth="1"/>
-    <col min="19" max="19" width="18.21875" customWidth="1"/>
+    <col min="3" max="4" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.33203125" customWidth="1"/>
+    <col min="6" max="6" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.33203125" customWidth="1"/>
+    <col min="8" max="10" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="3.33203125" customWidth="1"/>
+    <col min="13" max="13" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.109375" customWidth="1"/>
+    <col min="19" max="19" width="24.5546875" customWidth="1"/>
+    <col min="20" max="20" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:18" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:18" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:18" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:23" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:23" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1476,35 +1484,41 @@
         <v>3</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="K9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="L9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="M9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:18" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Q9" s="1"/>
+      <c r="V9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" cm="1">
         <f t="array" ref="B10:B40">_xlfn.SEQUENCE(31)</f>
         <v>1</v>
@@ -1516,17 +1530,25 @@
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
-      <c r="J10" s="15"/>
+      <c r="J10" s="9"/>
       <c r="K10" s="15"/>
-      <c r="L10" s="10"/>
-      <c r="Q10" t="s">
+      <c r="L10" s="15"/>
+      <c r="M10" s="10"/>
+      <c r="R10" t="s">
         <v>32</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V10" t="str" cm="1">
+        <f t="array" ref="V10:W80">_xlfn.LET(_xlpm.nums,_xlfn.SEQUENCE(70,,128522),_xlfn.VSTACK({"UNICODE value","emoji from UNICHAR"},_xlfn.HSTACK(_xlpm.nums,_xlfn.UNICHAR(_xlpm.nums))))</f>
+        <v>UNICODE value</v>
+      </c>
+      <c r="W10" t="str">
+        <v>emoji from UNICHAR</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>2</v>
       </c>
@@ -1537,17 +1559,24 @@
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="15"/>
+      <c r="J11" s="9"/>
       <c r="K11" s="15"/>
-      <c r="L11" s="10"/>
-      <c r="Q11" t="s">
+      <c r="L11" s="15"/>
+      <c r="M11" s="10"/>
+      <c r="R11" t="s">
         <v>10</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V11">
+        <v>128522</v>
+      </c>
+      <c r="W11" t="str">
+        <v>😊</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>3</v>
       </c>
@@ -1558,17 +1587,24 @@
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="15"/>
+      <c r="J12" s="9"/>
       <c r="K12" s="15"/>
-      <c r="L12" s="10"/>
-      <c r="Q12" t="s">
+      <c r="L12" s="15"/>
+      <c r="M12" s="10"/>
+      <c r="R12" t="s">
         <v>12</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V12">
+        <v>128523</v>
+      </c>
+      <c r="W12" t="str">
+        <v>😋</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>4</v>
       </c>
@@ -1579,17 +1615,24 @@
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="15"/>
+      <c r="J13" s="9"/>
       <c r="K13" s="15"/>
-      <c r="L13" s="10"/>
-      <c r="Q13" t="s">
+      <c r="L13" s="15"/>
+      <c r="M13" s="10"/>
+      <c r="R13" t="s">
         <v>14</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V13">
+        <v>128524</v>
+      </c>
+      <c r="W13" t="str">
+        <v>😌</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>5</v>
       </c>
@@ -1600,17 +1643,24 @@
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="15"/>
+      <c r="J14" s="9"/>
       <c r="K14" s="15"/>
-      <c r="L14" s="10"/>
-      <c r="Q14" t="s">
+      <c r="L14" s="15"/>
+      <c r="M14" s="10"/>
+      <c r="R14" t="s">
         <v>15</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V14">
+        <v>128525</v>
+      </c>
+      <c r="W14" t="str">
+        <v>😍</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>6</v>
       </c>
@@ -1621,17 +1671,24 @@
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
-      <c r="J15" s="15"/>
+      <c r="J15" s="9"/>
       <c r="K15" s="15"/>
-      <c r="L15" s="10"/>
-      <c r="Q15" t="s">
+      <c r="L15" s="15"/>
+      <c r="M15" s="10"/>
+      <c r="R15" t="s">
         <v>17</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V15">
+        <v>128526</v>
+      </c>
+      <c r="W15" t="str">
+        <v>😎</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <v>7</v>
       </c>
@@ -1642,17 +1699,24 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
-      <c r="J16" s="15"/>
+      <c r="J16" s="9"/>
       <c r="K16" s="15"/>
-      <c r="L16" s="10"/>
-      <c r="Q16" t="s">
+      <c r="L16" s="15"/>
+      <c r="M16" s="10"/>
+      <c r="R16" t="s">
         <v>19</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V16">
+        <v>128527</v>
+      </c>
+      <c r="W16" t="str">
+        <v>😏</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>8</v>
       </c>
@@ -1663,17 +1727,24 @@
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="15"/>
+      <c r="J17" s="9"/>
       <c r="K17" s="15"/>
-      <c r="L17" s="10"/>
-      <c r="Q17" t="s">
+      <c r="L17" s="15"/>
+      <c r="M17" s="10"/>
+      <c r="R17" t="s">
         <v>21</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V17">
+        <v>128528</v>
+      </c>
+      <c r="W17" t="str">
+        <v>😐</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <v>9</v>
       </c>
@@ -1684,17 +1755,24 @@
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
-      <c r="J18" s="15"/>
+      <c r="J18" s="9"/>
       <c r="K18" s="15"/>
-      <c r="L18" s="10"/>
-      <c r="Q18" t="s">
+      <c r="L18" s="15"/>
+      <c r="M18" s="10"/>
+      <c r="R18" t="s">
         <v>23</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V18">
+        <v>128529</v>
+      </c>
+      <c r="W18" t="str">
+        <v>😑</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>10</v>
       </c>
@@ -1705,17 +1783,24 @@
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
-      <c r="J19" s="15"/>
+      <c r="J19" s="9"/>
       <c r="K19" s="15"/>
-      <c r="L19" s="10"/>
-      <c r="Q19" t="s">
+      <c r="L19" s="15"/>
+      <c r="M19" s="10"/>
+      <c r="R19" t="s">
         <v>25</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V19">
+        <v>128530</v>
+      </c>
+      <c r="W19" t="str">
+        <v>😒</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B20" s="5">
         <v>11</v>
       </c>
@@ -1726,17 +1811,24 @@
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="15"/>
+      <c r="J20" s="9"/>
       <c r="K20" s="15"/>
-      <c r="L20" s="10"/>
-      <c r="Q20" t="s">
+      <c r="L20" s="15"/>
+      <c r="M20" s="10"/>
+      <c r="R20" t="s">
         <v>27</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V20">
+        <v>128531</v>
+      </c>
+      <c r="W20" t="str">
+        <v>😓</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B21" s="5">
         <v>12</v>
       </c>
@@ -1746,10 +1838,10 @@
       <c r="D21" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="E21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="9"/>
       <c r="G21" s="9" t="s">
         <v>9</v>
       </c>
@@ -1759,19 +1851,28 @@
       <c r="I21" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J21" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="K21" s="15"/>
-      <c r="L21" s="10"/>
-      <c r="Q21" t="s">
+      <c r="J21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21" s="15"/>
+      <c r="M21" s="10"/>
+      <c r="R21" t="s">
         <v>29</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V21">
+        <v>128532</v>
+      </c>
+      <c r="W21" t="str">
+        <v>😔</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B22" s="5">
         <v>13</v>
       </c>
@@ -1781,10 +1882,10 @@
       <c r="D22" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="E22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="9"/>
       <c r="G22" s="9" t="s">
         <v>9</v>
       </c>
@@ -1794,15 +1895,24 @@
       <c r="I22" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J22" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="K22" s="15"/>
-      <c r="L22" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="J22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="L22" s="15"/>
+      <c r="M22" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="V22">
+        <v>128533</v>
+      </c>
+      <c r="W22" t="str">
+        <v>😕</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
         <v>14</v>
       </c>
@@ -1827,41 +1937,77 @@
       <c r="I23" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J23" s="15" t="s">
+      <c r="J23" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K23" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="L23" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="L23" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="M23" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="V23">
+        <v>128534</v>
+      </c>
+      <c r="W23" t="str">
+        <v>😖</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B24" s="5">
         <v>15</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
+      <c r="C24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="I24" s="9"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="10"/>
-      <c r="Q24" t="s">
+      <c r="J24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="M24" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="R24" t="s">
         <v>37</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>38</v>
       </c>
-      <c r="S24" t="s">
+      <c r="T24" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V24">
+        <v>128535</v>
+      </c>
+      <c r="W24" t="str">
+        <v>😗</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
         <v>16</v>
       </c>
@@ -1872,20 +2018,27 @@
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
-      <c r="J25" s="15"/>
+      <c r="J25" s="9"/>
       <c r="K25" s="15"/>
-      <c r="L25" s="10"/>
-      <c r="Q25" t="s">
+      <c r="L25" s="15"/>
+      <c r="M25" s="10"/>
+      <c r="R25" t="s">
         <v>39</v>
       </c>
-      <c r="R25" t="s">
+      <c r="S25" t="s">
         <v>40</v>
       </c>
-      <c r="S25" t="s">
+      <c r="T25" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V25">
+        <v>128536</v>
+      </c>
+      <c r="W25" t="str">
+        <v>😘</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
         <v>17</v>
       </c>
@@ -1896,20 +2049,27 @@
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
-      <c r="J26" s="15"/>
+      <c r="J26" s="9"/>
       <c r="K26" s="15"/>
-      <c r="L26" s="10"/>
-      <c r="Q26" t="s">
+      <c r="L26" s="15"/>
+      <c r="M26" s="10"/>
+      <c r="R26" t="s">
         <v>41</v>
       </c>
-      <c r="R26" t="s">
+      <c r="S26" t="s">
         <v>42</v>
       </c>
-      <c r="S26" t="s">
+      <c r="T26" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V26">
+        <v>128537</v>
+      </c>
+      <c r="W26" t="str">
+        <v>😙</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
         <v>18</v>
       </c>
@@ -1920,20 +2080,27 @@
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="15"/>
+      <c r="J27" s="9"/>
       <c r="K27" s="15"/>
-      <c r="L27" s="10"/>
-      <c r="Q27" t="s">
+      <c r="L27" s="15"/>
+      <c r="M27" s="10"/>
+      <c r="R27" t="s">
         <v>43</v>
       </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>44</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V27">
+        <v>128538</v>
+      </c>
+      <c r="W27" t="str">
+        <v>😚</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
         <v>19</v>
       </c>
@@ -1944,20 +2111,27 @@
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
-      <c r="J28" s="15"/>
+      <c r="J28" s="9"/>
       <c r="K28" s="15"/>
-      <c r="L28" s="10"/>
-      <c r="Q28" t="s">
+      <c r="L28" s="15"/>
+      <c r="M28" s="10"/>
+      <c r="R28" t="s">
         <v>45</v>
       </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>46</v>
       </c>
-      <c r="S28" t="s">
+      <c r="T28" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V28">
+        <v>128539</v>
+      </c>
+      <c r="W28" t="str">
+        <v>😛</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B29" s="5">
         <v>20</v>
       </c>
@@ -1968,20 +2142,27 @@
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="15"/>
+      <c r="J29" s="9"/>
       <c r="K29" s="15"/>
-      <c r="L29" s="10"/>
-      <c r="Q29" t="s">
+      <c r="L29" s="15"/>
+      <c r="M29" s="10"/>
+      <c r="R29" t="s">
         <v>47</v>
       </c>
-      <c r="R29" t="s">
+      <c r="S29" t="s">
         <v>48</v>
       </c>
-      <c r="S29" t="s">
+      <c r="T29" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V29">
+        <v>128540</v>
+      </c>
+      <c r="W29" t="str">
+        <v>😜</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B30" s="5">
         <v>21</v>
       </c>
@@ -1992,20 +2173,27 @@
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
-      <c r="J30" s="15"/>
+      <c r="J30" s="9"/>
       <c r="K30" s="15"/>
-      <c r="L30" s="10"/>
-      <c r="Q30" t="s">
+      <c r="L30" s="15"/>
+      <c r="M30" s="10"/>
+      <c r="R30" t="s">
         <v>49</v>
       </c>
-      <c r="R30" t="s">
+      <c r="S30" t="s">
         <v>50</v>
       </c>
-      <c r="S30" t="s">
+      <c r="T30" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V30">
+        <v>128541</v>
+      </c>
+      <c r="W30" t="str">
+        <v>😝</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B31" s="5">
         <v>22</v>
       </c>
@@ -2016,20 +2204,27 @@
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
-      <c r="J31" s="15"/>
+      <c r="J31" s="9"/>
       <c r="K31" s="15"/>
-      <c r="L31" s="10"/>
-      <c r="Q31" t="s">
+      <c r="L31" s="15"/>
+      <c r="M31" s="10"/>
+      <c r="R31" t="s">
         <v>51</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>52</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V31">
+        <v>128542</v>
+      </c>
+      <c r="W31" t="str">
+        <v>😞</v>
+      </c>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B32" s="5">
         <v>23</v>
       </c>
@@ -2040,20 +2235,27 @@
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
-      <c r="J32" s="15"/>
+      <c r="J32" s="9"/>
       <c r="K32" s="15"/>
-      <c r="L32" s="10"/>
-      <c r="Q32" t="s">
+      <c r="L32" s="15"/>
+      <c r="M32" s="10"/>
+      <c r="R32" t="s">
         <v>53</v>
       </c>
-      <c r="R32" t="s">
+      <c r="S32" t="s">
         <v>54</v>
       </c>
-      <c r="S32" t="s">
+      <c r="T32" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V32">
+        <v>128543</v>
+      </c>
+      <c r="W32" t="str">
+        <v>😟</v>
+      </c>
+    </row>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B33" s="5">
         <v>24</v>
       </c>
@@ -2064,20 +2266,27 @@
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
-      <c r="J33" s="15"/>
+      <c r="J33" s="9"/>
       <c r="K33" s="15"/>
-      <c r="L33" s="10"/>
-      <c r="Q33" t="s">
+      <c r="L33" s="15"/>
+      <c r="M33" s="10"/>
+      <c r="R33" t="s">
         <v>55</v>
       </c>
-      <c r="R33" t="s">
+      <c r="S33" t="s">
         <v>56</v>
       </c>
-      <c r="S33" t="s">
+      <c r="T33" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V33">
+        <v>128544</v>
+      </c>
+      <c r="W33" t="str">
+        <v>😠</v>
+      </c>
+    </row>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B34" s="5">
         <v>25</v>
       </c>
@@ -2088,20 +2297,27 @@
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
-      <c r="J34" s="15"/>
+      <c r="J34" s="9"/>
       <c r="K34" s="15"/>
-      <c r="L34" s="10"/>
-      <c r="Q34" t="s">
+      <c r="L34" s="15"/>
+      <c r="M34" s="10"/>
+      <c r="R34" t="s">
         <v>57</v>
       </c>
-      <c r="R34" t="s">
+      <c r="S34" t="s">
         <v>58</v>
       </c>
-      <c r="S34" t="s">
+      <c r="T34" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V34">
+        <v>128545</v>
+      </c>
+      <c r="W34" t="str">
+        <v>😡</v>
+      </c>
+    </row>
+    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B35" s="5">
         <v>26</v>
       </c>
@@ -2112,20 +2328,27 @@
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
-      <c r="J35" s="15"/>
+      <c r="J35" s="9"/>
       <c r="K35" s="15"/>
-      <c r="L35" s="10"/>
-      <c r="Q35" t="s">
+      <c r="L35" s="15"/>
+      <c r="M35" s="10"/>
+      <c r="R35" t="s">
         <v>59</v>
       </c>
-      <c r="R35" t="s">
+      <c r="S35" t="s">
         <v>60</v>
       </c>
-      <c r="S35" t="s">
+      <c r="T35" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V35">
+        <v>128546</v>
+      </c>
+      <c r="W35" t="str">
+        <v>😢</v>
+      </c>
+    </row>
+    <row r="36" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B36" s="5">
         <v>27</v>
       </c>
@@ -2136,20 +2359,27 @@
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
-      <c r="J36" s="15"/>
+      <c r="J36" s="9"/>
       <c r="K36" s="15"/>
-      <c r="L36" s="10"/>
-      <c r="Q36" t="s">
+      <c r="L36" s="15"/>
+      <c r="M36" s="10"/>
+      <c r="R36" t="s">
         <v>61</v>
       </c>
-      <c r="R36" t="s">
+      <c r="S36" t="s">
         <v>62</v>
       </c>
-      <c r="S36" t="s">
+      <c r="T36" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V36">
+        <v>128547</v>
+      </c>
+      <c r="W36" t="str">
+        <v>😣</v>
+      </c>
+    </row>
+    <row r="37" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B37" s="5">
         <v>28</v>
       </c>
@@ -2160,20 +2390,27 @@
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
       <c r="I37" s="9"/>
-      <c r="J37" s="15"/>
+      <c r="J37" s="9"/>
       <c r="K37" s="15"/>
-      <c r="L37" s="10"/>
-      <c r="Q37" t="s">
+      <c r="L37" s="15"/>
+      <c r="M37" s="10"/>
+      <c r="R37" t="s">
         <v>63</v>
       </c>
-      <c r="R37" t="s">
+      <c r="S37" t="s">
         <v>64</v>
       </c>
-      <c r="S37" t="s">
+      <c r="T37" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V37">
+        <v>128548</v>
+      </c>
+      <c r="W37" t="str">
+        <v>😤</v>
+      </c>
+    </row>
+    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B38" s="5">
         <v>29</v>
       </c>
@@ -2184,20 +2421,27 @@
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
-      <c r="J38" s="15"/>
+      <c r="J38" s="9"/>
       <c r="K38" s="15"/>
-      <c r="L38" s="10"/>
-      <c r="Q38" t="s">
+      <c r="L38" s="15"/>
+      <c r="M38" s="10"/>
+      <c r="R38" t="s">
         <v>65</v>
       </c>
-      <c r="R38" t="s">
+      <c r="S38" t="s">
         <v>66</v>
       </c>
-      <c r="S38" t="s">
+      <c r="T38" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V38">
+        <v>128549</v>
+      </c>
+      <c r="W38" t="str">
+        <v>😥</v>
+      </c>
+    </row>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B39" s="5">
         <v>30</v>
       </c>
@@ -2208,20 +2452,27 @@
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
-      <c r="J39" s="15"/>
+      <c r="J39" s="9"/>
       <c r="K39" s="15"/>
-      <c r="L39" s="10"/>
-      <c r="Q39" t="s">
+      <c r="L39" s="15"/>
+      <c r="M39" s="10"/>
+      <c r="R39" t="s">
         <v>67</v>
       </c>
-      <c r="R39" t="s">
+      <c r="S39" t="s">
         <v>68</v>
       </c>
-      <c r="S39" t="s">
+      <c r="T39" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="40" spans="2:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V39">
+        <v>128550</v>
+      </c>
+      <c r="W39" t="str">
+        <v>😦</v>
+      </c>
+    </row>
+    <row r="40" spans="2:23" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="6">
         <v>31</v>
       </c>
@@ -2232,46 +2483,369 @@
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
-      <c r="J40" s="16"/>
+      <c r="J40" s="12"/>
       <c r="K40" s="16"/>
-      <c r="L40" s="13"/>
-      <c r="Q40" t="s">
+      <c r="L40" s="16"/>
+      <c r="M40" s="13"/>
+      <c r="R40" t="s">
         <v>69</v>
       </c>
-      <c r="R40" t="s">
+      <c r="S40" t="s">
         <v>70</v>
       </c>
-      <c r="S40" t="s">
+      <c r="T40" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="Q41" t="s">
+      <c r="V40">
+        <v>128551</v>
+      </c>
+      <c r="W40" t="str">
+        <v>😧</v>
+      </c>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="R41" t="s">
         <v>71</v>
       </c>
-      <c r="R41" t="s">
+      <c r="S41" t="s">
         <v>72</v>
       </c>
-      <c r="S41" t="s">
+      <c r="T41" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="Q42" t="s">
+      <c r="V41">
+        <v>128552</v>
+      </c>
+      <c r="W41" t="str">
+        <v>😨</v>
+      </c>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="R42" t="s">
         <v>73</v>
       </c>
-      <c r="R42" t="s">
+      <c r="S42" t="s">
         <v>74</v>
       </c>
-      <c r="S42" t="s">
+      <c r="T42" t="s">
         <v>91</v>
       </c>
+      <c r="V42">
+        <v>128553</v>
+      </c>
+      <c r="W42" t="str">
+        <v>😩</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V43">
+        <v>128554</v>
+      </c>
+      <c r="W43" t="str">
+        <v>😪</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V44">
+        <v>128555</v>
+      </c>
+      <c r="W44" t="str">
+        <v>😫</v>
+      </c>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V45">
+        <v>128556</v>
+      </c>
+      <c r="W45" t="str">
+        <v>😬</v>
+      </c>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V46">
+        <v>128557</v>
+      </c>
+      <c r="W46" t="str">
+        <v>😭</v>
+      </c>
+    </row>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V47">
+        <v>128558</v>
+      </c>
+      <c r="W47" t="str">
+        <v>😮</v>
+      </c>
+    </row>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V48">
+        <v>128559</v>
+      </c>
+      <c r="W48" t="str">
+        <v>😯</v>
+      </c>
+    </row>
+    <row r="49" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V49">
+        <v>128560</v>
+      </c>
+      <c r="W49" t="str">
+        <v>😰</v>
+      </c>
+    </row>
+    <row r="50" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V50">
+        <v>128561</v>
+      </c>
+      <c r="W50" t="str">
+        <v>😱</v>
+      </c>
+    </row>
+    <row r="51" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V51">
+        <v>128562</v>
+      </c>
+      <c r="W51" t="str">
+        <v>😲</v>
+      </c>
+    </row>
+    <row r="52" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V52">
+        <v>128563</v>
+      </c>
+      <c r="W52" t="str">
+        <v>😳</v>
+      </c>
+    </row>
+    <row r="53" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V53">
+        <v>128564</v>
+      </c>
+      <c r="W53" t="str">
+        <v>😴</v>
+      </c>
+    </row>
+    <row r="54" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V54">
+        <v>128565</v>
+      </c>
+      <c r="W54" t="str">
+        <v>😵</v>
+      </c>
+    </row>
+    <row r="55" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V55">
+        <v>128566</v>
+      </c>
+      <c r="W55" t="str">
+        <v>😶</v>
+      </c>
+    </row>
+    <row r="56" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V56">
+        <v>128567</v>
+      </c>
+      <c r="W56" t="str">
+        <v>😷</v>
+      </c>
+    </row>
+    <row r="57" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V57">
+        <v>128568</v>
+      </c>
+      <c r="W57" t="str">
+        <v>😸</v>
+      </c>
+    </row>
+    <row r="58" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V58">
+        <v>128569</v>
+      </c>
+      <c r="W58" t="str">
+        <v>😹</v>
+      </c>
+    </row>
+    <row r="59" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V59">
+        <v>128570</v>
+      </c>
+      <c r="W59" t="str">
+        <v>😺</v>
+      </c>
+    </row>
+    <row r="60" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V60">
+        <v>128571</v>
+      </c>
+      <c r="W60" t="str">
+        <v>😻</v>
+      </c>
+    </row>
+    <row r="61" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V61">
+        <v>128572</v>
+      </c>
+      <c r="W61" t="str">
+        <v>😼</v>
+      </c>
+    </row>
+    <row r="62" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V62">
+        <v>128573</v>
+      </c>
+      <c r="W62" t="str">
+        <v>😽</v>
+      </c>
+    </row>
+    <row r="63" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V63">
+        <v>128574</v>
+      </c>
+      <c r="W63" t="str">
+        <v>😾</v>
+      </c>
+    </row>
+    <row r="64" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V64">
+        <v>128575</v>
+      </c>
+      <c r="W64" t="str">
+        <v>😿</v>
+      </c>
+    </row>
+    <row r="65" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V65">
+        <v>128576</v>
+      </c>
+      <c r="W65" t="str">
+        <v>🙀</v>
+      </c>
+    </row>
+    <row r="66" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V66">
+        <v>128577</v>
+      </c>
+      <c r="W66" t="str">
+        <v>🙁</v>
+      </c>
+    </row>
+    <row r="67" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V67">
+        <v>128578</v>
+      </c>
+      <c r="W67" t="str">
+        <v>🙂</v>
+      </c>
+    </row>
+    <row r="68" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V68">
+        <v>128579</v>
+      </c>
+      <c r="W68" t="str">
+        <v>🙃</v>
+      </c>
+    </row>
+    <row r="69" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V69">
+        <v>128580</v>
+      </c>
+      <c r="W69" t="str">
+        <v>🙄</v>
+      </c>
+    </row>
+    <row r="70" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V70">
+        <v>128581</v>
+      </c>
+      <c r="W70" t="str">
+        <v>🙅</v>
+      </c>
+    </row>
+    <row r="71" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V71">
+        <v>128582</v>
+      </c>
+      <c r="W71" t="str">
+        <v>🙆</v>
+      </c>
+    </row>
+    <row r="72" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V72">
+        <v>128583</v>
+      </c>
+      <c r="W72" t="str">
+        <v>🙇</v>
+      </c>
+    </row>
+    <row r="73" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V73">
+        <v>128584</v>
+      </c>
+      <c r="W73" t="str">
+        <v>🙈</v>
+      </c>
+    </row>
+    <row r="74" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V74">
+        <v>128585</v>
+      </c>
+      <c r="W74" t="str">
+        <v>🙉</v>
+      </c>
+    </row>
+    <row r="75" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V75">
+        <v>128586</v>
+      </c>
+      <c r="W75" t="str">
+        <v>🙊</v>
+      </c>
+    </row>
+    <row r="76" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V76">
+        <v>128587</v>
+      </c>
+      <c r="W76" t="str">
+        <v>🙋</v>
+      </c>
+    </row>
+    <row r="77" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V77">
+        <v>128588</v>
+      </c>
+      <c r="W77" t="str">
+        <v>🙌</v>
+      </c>
+    </row>
+    <row r="78" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V78">
+        <v>128589</v>
+      </c>
+      <c r="W78" t="str">
+        <v>🙍</v>
+      </c>
+    </row>
+    <row r="79" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V79">
+        <v>128590</v>
+      </c>
+      <c r="W79" t="str">
+        <v>🙎</v>
+      </c>
+    </row>
+    <row r="80" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V80">
+        <v>128591</v>
+      </c>
+      <c r="W80" t="str">
+        <v>🙏</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="S24:S60">
-    <sortCondition ref="S24:S60"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="T24:T60">
+    <sortCondition ref="T24:T60"/>
   </sortState>
-  <conditionalFormatting sqref="B10:L40">
+  <conditionalFormatting sqref="B10:M40">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(B10)-ROW($B$9),2)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Today's status. I am up at the cabin late and no time to weight lift
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFDF63F-221E-43AC-9ADA-963A630463C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418D1835-6E2E-4F1E-963A-681F73CEC57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="96">
   <si>
     <t>Day</t>
   </si>
@@ -1453,9 +1453,9 @@
   <dimension ref="A7:W80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomLeft" activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2329,17 +2329,37 @@
       <c r="B31" s="5">
         <v>22</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
+      <c r="C31" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="10"/>
+      <c r="G31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K31" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="L31" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="M31" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="R31" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
Cared for CJ today. Did the minimum
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28604"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB17EAEC-7F4B-4CF7-B607-DF0C992012C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811BA1B2-FB59-4497-B6C0-8A7EEE04C348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="99">
   <si>
     <t>Day</t>
   </si>
@@ -1472,7 +1472,7 @@
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
+      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3105,7 +3105,9 @@
       <c r="D46" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E46" s="7"/>
+      <c r="E46" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="F46" s="7"/>
       <c r="G46" s="7" t="s">
         <v>9</v>
@@ -3139,17 +3141,37 @@
       <c r="B47" s="16" t="str">
         <v>07-Feb</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
+      <c r="C47" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="13"/>
-      <c r="M47" s="8"/>
+      <c r="G47" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K47" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M47" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="V47">
         <v>128558</v>
       </c>

</xml_diff>

<commit_message>
Put banded rows in report
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D3FF0E-65B3-46E5-8ACB-1B8EA4F298D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375BAA5B-E8AC-4F83-9C2A-8744A193A73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -19,6 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$R$24:$R$60</definedName>
     <definedName name="Banded">_xlfn.DROP(_xlfn._TRO_ALL(Report!$B:$N),1)</definedName>
+    <definedName name="Banded2">_xlfn.DROP(_xlfn._TRO_ALL(Report!$R:$AD),1)</definedName>
     <definedName name="data">_xlfn.TRIMRANGE(Report!B20:N999,2)</definedName>
     <definedName name="fmt" localSheetId="0">_xlfn.DROP(_xlfn._TRO_ALL(Report!$C:$N),12)</definedName>
     <definedName name="fmt" localSheetId="1">_xlfn._TRO_ALL(Summary!$A:$M)</definedName>
@@ -624,7 +625,21 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -878,27 +893,27 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Standard Pivot Table" table="0" count="12" xr9:uid="{94886349-6B4A-4300-89B0-9F83C8B5183A}">
-      <tableStyleElement type="wholeTable" dxfId="21"/>
-      <tableStyleElement type="headerRow" dxfId="20"/>
-      <tableStyleElement type="totalRow" dxfId="19"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="18"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="17"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="16"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="15"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="14"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="13"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="12"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="11"/>
-      <tableStyleElement type="pageFieldValues" dxfId="10"/>
+      <tableStyleElement type="wholeTable" dxfId="23"/>
+      <tableStyleElement type="headerRow" dxfId="22"/>
+      <tableStyleElement type="totalRow" dxfId="21"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="20"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="19"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="18"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="17"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="16"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="15"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="14"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="13"/>
+      <tableStyleElement type="pageFieldValues" dxfId="12"/>
     </tableStyle>
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="9"/>
-      <tableStyleElement type="headerRow" dxfId="8"/>
-      <tableStyleElement type="totalRow" dxfId="7"/>
-      <tableStyleElement type="firstColumn" dxfId="6"/>
-      <tableStyleElement type="lastColumn" dxfId="5"/>
-      <tableStyleElement type="firstRowStripe" dxfId="4"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="3"/>
+      <tableStyleElement type="wholeTable" dxfId="11"/>
+      <tableStyleElement type="headerRow" dxfId="10"/>
+      <tableStyleElement type="totalRow" dxfId="9"/>
+      <tableStyleElement type="firstColumn" dxfId="8"/>
+      <tableStyleElement type="lastColumn" dxfId="7"/>
+      <tableStyleElement type="firstRowStripe" dxfId="6"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="5"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1251,9 +1266,9 @@
   <dimension ref="A7:AD68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="AG26" sqref="AG26"/>
+      <selection pane="bottomLeft" activeCell="AH5" sqref="AH5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1268,9 +1283,9 @@
     <col min="19" max="30" width="3.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:17" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:17" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:17" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:30" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:30" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1316,8 +1331,47 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="R9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="S9" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD9" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="str" cm="1">
         <f t="array" aca="1" ref="B10:B55" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
         <v>01-Jan</v>
@@ -1338,8 +1392,60 @@
         <f ca="1">WEEKNUM(B10)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R10" s="24" cm="1">
+        <f t="array" aca="1" ref="R10:AD14" ca="1">_xlfn.PIVOTBY(O21:O55,,fmt,_xleta.SUM,0,0)</f>
+        <v>3</v>
+      </c>
+      <c r="S10">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="T10">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="U10">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="V10">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="W10">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="X10">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="Y10">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="Z10">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AA10">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AB10">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="AC10">
+        <f ca="1"/>
+        <v>6</v>
+      </c>
+      <c r="AD10">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="str">
         <f ca="1"/>
         <v>02-Jan</v>
@@ -1360,8 +1466,60 @@
         <f t="shared" ref="O11:O55" ca="1" si="0">WEEKNUM(B11)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11" s="24">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="T11">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="U11">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="V11">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="W11">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="X11">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="Y11">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="Z11">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AA11">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AB11">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AC11">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AD11">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="str">
         <f ca="1"/>
         <v>03-Jan</v>
@@ -1382,8 +1540,60 @@
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12" s="24">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="S12">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="T12">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="U12">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="V12">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="W12">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="X12">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="Y12">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="Z12">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AA12">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AB12">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AC12">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AD12">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="str">
         <f ca="1"/>
         <v>04-Jan</v>
@@ -1404,8 +1614,60 @@
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13" s="24">
+        <f ca="1"/>
+        <v>6</v>
+      </c>
+      <c r="S13">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="T13">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="V13">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="W13">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="X13">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="Y13">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="Z13">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AA13">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AB13">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AC13">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AD13">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="str">
         <f ca="1"/>
         <v>05-Jan</v>
@@ -1426,8 +1688,60 @@
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14" s="24">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="S14">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="V14">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="W14">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="X14">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="Y14">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="Z14">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AA14">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AB14">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AC14">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="AD14">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="str">
         <f ca="1"/>
         <v>06-Jan</v>
@@ -1449,7 +1763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="str">
         <f ca="1"/>
         <v>07-Jan</v>
@@ -1471,7 +1785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="str">
         <f ca="1"/>
         <v>08-Jan</v>
@@ -1493,7 +1807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="str">
         <f ca="1"/>
         <v>09-Jan</v>
@@ -1515,7 +1829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="str">
         <f ca="1"/>
         <v>10-Jan</v>
@@ -1537,7 +1851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="str">
         <f ca="1"/>
         <v>11-Jan</v>
@@ -1560,7 +1874,7 @@
       </c>
       <c r="S20" s="21"/>
     </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="str">
         <f ca="1"/>
         <v>12-Jan</v>
@@ -1610,7 +1924,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="str">
         <f ca="1"/>
         <v>13-Jan</v>
@@ -1660,7 +1974,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" s="13" t="str">
         <f ca="1"/>
         <v>14-Jan</v>
@@ -1710,7 +2024,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24" s="13" t="str">
         <f ca="1"/>
         <v>15-Jan</v>
@@ -1760,7 +2074,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:30" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B25" s="13" t="str">
         <f ca="1"/>
         <v>16-Jan</v>
@@ -1810,7 +2124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="2:30" ht="121.2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B26" s="13" t="str">
         <f ca="1"/>
         <v>17-Jan</v>
@@ -1859,47 +2173,8 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="R26" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="S26" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="T26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="U26" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="V26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="W26" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="X26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA26" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB26" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD26" s="15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="2:30" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B27" s="13" t="str">
         <f ca="1"/>
         <v>18-Jan</v>
@@ -1948,60 +2223,8 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="R27" s="24" cm="1">
-        <f t="array" aca="1" ref="R27:AD31" ca="1">_xlfn.PIVOTBY(O21:O55,,fmt,_xleta.SUM,0,0)</f>
-        <v>3</v>
-      </c>
-      <c r="S27">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="T27">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="U27">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="V27">
-        <f ca="1"/>
-        <v>4</v>
-      </c>
-      <c r="W27">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="X27">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="Y27">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="Z27">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AA27">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AB27">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="AC27">
-        <f ca="1"/>
-        <v>6</v>
-      </c>
-      <c r="AD27">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B28" s="13" t="str">
         <f ca="1"/>
         <v>19-Jan</v>
@@ -2050,60 +2273,8 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="R28" s="24">
-        <f ca="1"/>
-        <v>4</v>
-      </c>
-      <c r="S28">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="T28">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="U28">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="V28">
-        <f ca="1"/>
-        <v>4</v>
-      </c>
-      <c r="W28">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="X28">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="Y28">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="Z28">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AA28">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AB28">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AC28">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AD28">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B29" s="13" t="str">
         <f ca="1"/>
         <v>20-Jan</v>
@@ -2152,60 +2323,8 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="R29" s="24">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="S29">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="T29">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="U29">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="V29">
-        <f ca="1"/>
-        <v>4</v>
-      </c>
-      <c r="W29">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="X29">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="Y29">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="Z29">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AA29">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AB29">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AC29">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AD29">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B30" s="13" t="str">
         <f ca="1"/>
         <v>21-Jan</v>
@@ -2254,60 +2373,8 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="R30" s="24">
-        <f ca="1"/>
-        <v>6</v>
-      </c>
-      <c r="S30">
-        <f ca="1"/>
-        <v>4</v>
-      </c>
-      <c r="T30">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="U30">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="V30">
-        <f ca="1"/>
-        <v>2</v>
-      </c>
-      <c r="W30">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="X30">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="Y30">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="Z30">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AA30">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AB30">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AC30">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AD30">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B31" s="13" t="str">
         <f ca="1"/>
         <v>22-Jan</v>
@@ -2356,60 +2423,8 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="R31" s="24">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="S31">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="T31">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="U31">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="V31">
-        <f ca="1"/>
-        <v>4</v>
-      </c>
-      <c r="W31">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="X31">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="Y31">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="Z31">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AA31">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AB31">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AC31">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
-      <c r="AD31">
-        <f ca="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B32" s="13" t="str">
         <f ca="1"/>
         <v>23-Jan</v>
@@ -3809,8 +3824,13 @@
     <sortCondition ref="T24:T60"/>
   </sortState>
   <conditionalFormatting sqref="B10:N55">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(B10)-ROW($B$9),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R10:AD14">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD(ROW(R10)-ROW($R$9),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6038,7 +6058,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:M35">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>MOD(ROW(A2)-ROW($A$1),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
List of deficiences added
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375BAA5B-E8AC-4F83-9C2A-8744A193A73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A225A4E-1E4E-4684-9B67-FF7202F20212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
   <si>
     <t>Day</t>
   </si>
@@ -129,6 +129,15 @@
   </si>
   <si>
     <t>Week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I need to come up with a general </t>
+  </si>
+  <si>
+    <t xml:space="preserve">format that allows me to complete </t>
+  </si>
+  <si>
+    <t>courses and not take a penalty.</t>
   </si>
 </sst>
 </file>
@@ -1263,12 +1272,12 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A7:AD68"/>
+  <dimension ref="A7:AG68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="AH5" sqref="AH5"/>
+      <selection pane="bottomLeft" activeCell="AG13" sqref="AG13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1283,9 +1292,9 @@
     <col min="19" max="30" width="3.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:30" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:30" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:30" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:33" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:33" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1371,7 +1380,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="str" cm="1">
         <f t="array" aca="1" ref="B10:B55" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
         <v>01-Jan</v>
@@ -1445,7 +1454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="str">
         <f ca="1"/>
         <v>02-Jan</v>
@@ -1518,8 +1527,11 @@
         <f ca="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AG11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="str">
         <f ca="1"/>
         <v>03-Jan</v>
@@ -1592,8 +1604,11 @@
         <f ca="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AG12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="str">
         <f ca="1"/>
         <v>04-Jan</v>
@@ -1666,8 +1681,11 @@
         <f ca="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AG13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="str">
         <f ca="1"/>
         <v>05-Jan</v>
@@ -1741,7 +1759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="str">
         <f ca="1"/>
         <v>06-Jan</v>
@@ -1763,7 +1781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="str">
         <f ca="1"/>
         <v>07-Jan</v>

</xml_diff>

<commit_message>
More work on reporting
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A225A4E-1E4E-4684-9B67-FF7202F20212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36324FC6-E676-48B2-9DC6-082D983337F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -20,10 +20,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$R$24:$R$60</definedName>
     <definedName name="Banded">_xlfn.DROP(_xlfn._TRO_ALL(Report!$B:$N),1)</definedName>
     <definedName name="Banded2">_xlfn.DROP(_xlfn._TRO_ALL(Report!$R:$AD),1)</definedName>
-    <definedName name="data">_xlfn.TRIMRANGE(Report!B20:N999,2)</definedName>
+    <definedName name="data">_xlfn.DROP(Banded,11,1)</definedName>
     <definedName name="fmt" localSheetId="0">_xlfn.DROP(_xlfn._TRO_ALL(Report!$C:$N),12)</definedName>
     <definedName name="fmt" localSheetId="1">_xlfn._TRO_ALL(Summary!$A:$M)</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
+    <definedName name="ix">_xlfn.DROP(_xlfn._TRO_ALL(Report!XFB:XFB),11)</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$B$9:$M$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -272,7 +273,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -529,6 +530,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -608,15 +620,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -634,28 +646,7 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <fill>
         <patternFill>
@@ -902,27 +893,27 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Standard Pivot Table" table="0" count="12" xr9:uid="{94886349-6B4A-4300-89B0-9F83C8B5183A}">
-      <tableStyleElement type="wholeTable" dxfId="23"/>
-      <tableStyleElement type="headerRow" dxfId="22"/>
-      <tableStyleElement type="totalRow" dxfId="21"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="20"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="19"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="18"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="17"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="16"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="15"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="14"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="13"/>
-      <tableStyleElement type="pageFieldValues" dxfId="12"/>
+      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="totalRow" dxfId="18"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="17"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="16"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="15"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="14"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="13"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="12"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="11"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="10"/>
+      <tableStyleElement type="pageFieldValues" dxfId="9"/>
     </tableStyle>
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="11"/>
-      <tableStyleElement type="headerRow" dxfId="10"/>
-      <tableStyleElement type="totalRow" dxfId="9"/>
-      <tableStyleElement type="firstColumn" dxfId="8"/>
-      <tableStyleElement type="lastColumn" dxfId="7"/>
-      <tableStyleElement type="firstRowStripe" dxfId="6"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="5"/>
+      <tableStyleElement type="wholeTable" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="7"/>
+      <tableStyleElement type="totalRow" dxfId="6"/>
+      <tableStyleElement type="firstColumn" dxfId="5"/>
+      <tableStyleElement type="lastColumn" dxfId="4"/>
+      <tableStyleElement type="firstRowStripe" dxfId="3"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1277,7 +1268,7 @@
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="AG13" sqref="AG13"/>
+      <selection pane="bottomLeft" activeCell="S52" sqref="S52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1340,10 +1331,10 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="25" t="s">
+      <c r="R9" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="S9" s="23" t="s">
+      <c r="S9" s="22" t="s">
         <v>2</v>
       </c>
       <c r="T9" s="3" t="s">
@@ -1382,7 +1373,7 @@
     </row>
     <row r="10" spans="1:33" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="str" cm="1">
-        <f t="array" aca="1" ref="B10:B55" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
+        <f t="array" aca="1" ref="B10:B56" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
         <v>01-Jan</v>
       </c>
       <c r="C10" s="5"/>
@@ -1401,8 +1392,8 @@
         <f ca="1">WEEKNUM(B10)</f>
         <v>1</v>
       </c>
-      <c r="R10" s="24" cm="1">
-        <f t="array" aca="1" ref="R10:AD14" ca="1">_xlfn.PIVOTBY(O21:O55,,fmt,_xleta.SUM,0,0)</f>
+      <c r="R10" s="23" cm="1">
+        <f t="array" aca="1" ref="R10:AD15" ca="1">_xlfn.PIVOTBY(ix,,data,_xleta.SUM,0,0)</f>
         <v>3</v>
       </c>
       <c r="S10">
@@ -1472,10 +1463,10 @@
       <c r="M11" s="6"/>
       <c r="N11" s="17"/>
       <c r="O11">
-        <f t="shared" ref="O11:O55" ca="1" si="0">WEEKNUM(B11)</f>
-        <v>1</v>
-      </c>
-      <c r="R11" s="24">
+        <f t="shared" ref="O11:O56" ca="1" si="0">WEEKNUM(B11)</f>
+        <v>1</v>
+      </c>
+      <c r="R11" s="23">
         <f ca="1"/>
         <v>4</v>
       </c>
@@ -1552,7 +1543,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-      <c r="R12" s="24">
+      <c r="R12" s="23">
         <f ca="1"/>
         <v>5</v>
       </c>
@@ -1629,7 +1620,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-      <c r="R13" s="24">
+      <c r="R13" s="23">
         <f ca="1"/>
         <v>6</v>
       </c>
@@ -1706,7 +1697,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="R14" s="24">
+      <c r="R14" s="23">
         <f ca="1"/>
         <v>7</v>
       </c>
@@ -1780,6 +1771,58 @@
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
+      <c r="R15" s="23">
+        <f ca="1"/>
+        <v>8</v>
+      </c>
+      <c r="S15">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="AD15">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="str">
@@ -1988,7 +2031,7 @@
         <v>3</v>
       </c>
       <c r="P22">
-        <f t="shared" ref="P22:P55" si="1">SUM(C22:N22)</f>
+        <f t="shared" ref="P22:P56" si="1">SUM(C22:N22)</f>
         <v>9</v>
       </c>
     </row>
@@ -3618,7 +3661,7 @@
       <c r="I55" s="6">
         <v>1</v>
       </c>
-      <c r="J55" s="22">
+      <c r="J55" s="6">
         <v>1</v>
       </c>
       <c r="K55" s="6">
@@ -3643,19 +3686,54 @@
       </c>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B56" s="13"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="6"/>
-      <c r="K56" s="10"/>
-      <c r="L56" s="10"/>
-      <c r="M56" s="6"/>
-      <c r="N56" s="17"/>
+      <c r="B56" s="13" t="str">
+        <f ca="1"/>
+        <v>16-Feb</v>
+      </c>
+      <c r="C56" s="5">
+        <v>0</v>
+      </c>
+      <c r="D56" s="6">
+        <v>0</v>
+      </c>
+      <c r="E56" s="6">
+        <v>0</v>
+      </c>
+      <c r="F56" s="6">
+        <v>0</v>
+      </c>
+      <c r="G56" s="6">
+        <v>0</v>
+      </c>
+      <c r="H56" s="6">
+        <v>0</v>
+      </c>
+      <c r="I56" s="6">
+        <v>0</v>
+      </c>
+      <c r="J56" s="6">
+        <v>0</v>
+      </c>
+      <c r="K56" s="6">
+        <v>0</v>
+      </c>
+      <c r="L56" s="6">
+        <v>0</v>
+      </c>
+      <c r="M56" s="6">
+        <v>1</v>
+      </c>
+      <c r="N56" s="25">
+        <v>1</v>
+      </c>
+      <c r="O56">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B57" s="13"/>
@@ -3841,14 +3919,19 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="T24:T60">
     <sortCondition ref="T24:T60"/>
   </sortState>
-  <conditionalFormatting sqref="B10:N55">
+  <conditionalFormatting sqref="B10:N56">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>MOD(ROW(B10)-ROW($B$9),2)</formula>
+      <formula>MOD(ROW(B10)-ROW($R$9),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R10:AD14">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>MOD(ROW(R10)-ROW($R$9),2)</formula>
+  <conditionalFormatting sqref="Q58">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3858,7 +3941,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9971042-F2FB-49FE-B9A5-F243354847EE}">
-  <dimension ref="A1:AD36"/>
+  <dimension ref="A1:AD37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
@@ -3909,189 +3992,142 @@
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="str" cm="1">
-        <f t="array" aca="1" ref="A2:M36" ca="1">data</f>
-        <v>12-Jan</v>
+      <c r="A2" s="16" cm="1">
+        <f t="array" ref="A2:L37">data</f>
+        <v>1</v>
       </c>
       <c r="B2" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="C2" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="D2" s="16">
-        <f ca="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="16">
-        <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="G2" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="H2" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="I2" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="J2" s="16">
-        <f ca="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="16">
-        <f ca="1"/>
         <v>0</v>
       </c>
       <c r="L2" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="M2" s="16">
-        <f ca="1"/>
         <v>0</v>
       </c>
       <c r="N2">
-        <f ca="1">WEEKNUM(A2)</f>
-        <v>3</v>
+        <f>WEEKNUM(A2)</f>
+        <v>1</v>
       </c>
       <c r="O2">
-        <f ca="1">SUM(B2:M2)</f>
+        <f>SUM(B2:M2)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16">
+        <v>1</v>
+      </c>
+      <c r="D3" s="16">
+        <v>0</v>
+      </c>
+      <c r="E3" s="16">
+        <v>1</v>
+      </c>
+      <c r="F3" s="16">
+        <v>1</v>
+      </c>
+      <c r="G3" s="16">
+        <v>1</v>
+      </c>
+      <c r="H3" s="16">
+        <v>1</v>
+      </c>
+      <c r="I3" s="16">
+        <v>1</v>
+      </c>
+      <c r="J3" s="16">
+        <v>0</v>
+      </c>
+      <c r="K3" s="16">
+        <v>1</v>
+      </c>
+      <c r="L3" s="16">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N35" si="0">WEEKNUM(A3)</f>
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O35" si="1">SUM(B3:M3)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="str">
-        <f ca="1"/>
-        <v>13-Jan</v>
-      </c>
-      <c r="B3" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="C3" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="D3" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E3" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F3" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G3" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H3" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I3" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J3" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K3" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="L3" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M3" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N35" ca="1" si="0">WEEKNUM(A3)</f>
-        <v>3</v>
-      </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O35" ca="1" si="1">SUM(B3:M3)</f>
-        <v>9</v>
-      </c>
-    </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="str">
-        <f ca="1"/>
-        <v>14-Jan</v>
+      <c r="A4" s="16">
+        <v>1</v>
       </c>
       <c r="B4" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="C4" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="D4" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="E4" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="F4" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="G4" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="H4" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="I4" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="J4" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="K4" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="L4" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M4" s="16">
-        <f ca="1"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="O4">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="Q4" t="e" cm="1" vm="1">
         <f t="array" ref="Q4">_xlfn.PIVOTBY(N2:N35,S1:AD1,B2:M35,_xleta.SUM)</f>
@@ -4099,1984 +4135,1510 @@
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="str">
-        <f ca="1"/>
-        <v>15-Jan</v>
+      <c r="A5" s="16">
+        <v>1</v>
       </c>
       <c r="B5" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="C5" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="D5" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="E5" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="F5" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="G5" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="H5" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="I5" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="J5" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="K5" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="L5" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M5" s="16">
-        <f ca="1"/>
         <v>0</v>
       </c>
       <c r="N5">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="O5">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="str">
-        <f ca="1"/>
-        <v>16-Jan</v>
+      <c r="A6" s="16">
+        <v>1</v>
       </c>
       <c r="B6" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="C6" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="D6" s="16">
-        <f ca="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="16">
-        <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="G6" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="H6" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="I6" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="J6" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="K6" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="L6" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M6" s="16">
-        <f ca="1"/>
         <v>0</v>
       </c>
       <c r="N6">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="O6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>1</v>
+      </c>
+      <c r="B7" s="16">
+        <v>1</v>
+      </c>
+      <c r="C7" s="16">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16">
+        <v>1</v>
+      </c>
+      <c r="E7" s="16">
+        <v>1</v>
+      </c>
+      <c r="F7" s="16">
+        <v>1</v>
+      </c>
+      <c r="G7" s="16">
+        <v>1</v>
+      </c>
+      <c r="H7" s="16">
+        <v>1</v>
+      </c>
+      <c r="I7" s="16">
+        <v>1</v>
+      </c>
+      <c r="J7" s="16">
+        <v>1</v>
+      </c>
+      <c r="K7" s="16">
+        <v>1</v>
+      </c>
+      <c r="L7" s="16">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="str">
-        <f ca="1"/>
-        <v>17-Jan</v>
-      </c>
-      <c r="B7" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="C7" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="D7" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E7" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="F7" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G7" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H7" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I7" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J7" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K7" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L7" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M7" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="O7">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
-      </c>
-    </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="str">
-        <f ca="1"/>
-        <v>18-Jan</v>
+      <c r="A8" s="16">
+        <v>1</v>
       </c>
       <c r="B8" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="C8" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="D8" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="E8" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="F8" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="G8" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="H8" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="I8" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="J8" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="K8" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="L8" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M8" s="16">
-        <f ca="1"/>
         <v>0</v>
       </c>
       <c r="N8">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="O8">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="str">
-        <f ca="1"/>
-        <v>19-Jan</v>
+      <c r="A9" s="16">
+        <v>1</v>
       </c>
       <c r="B9" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="C9" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="D9" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="E9" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="F9" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="G9" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="H9" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="I9" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="J9" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="K9" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="L9" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M9" s="16">
-        <f ca="1"/>
         <v>0</v>
       </c>
       <c r="N9">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="O9">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="str">
-        <f ca="1"/>
-        <v>20-Jan</v>
+      <c r="A10" s="16">
+        <v>1</v>
       </c>
       <c r="B10" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="C10" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="D10" s="16">
-        <f ca="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="16">
-        <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="G10" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="H10" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="I10" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="J10" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="K10" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="L10" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M10" s="16">
-        <f ca="1"/>
         <v>0</v>
       </c>
       <c r="N10">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="O10">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>1</v>
+      </c>
+      <c r="B11" s="16">
+        <v>1</v>
+      </c>
+      <c r="C11" s="16">
+        <v>1</v>
+      </c>
+      <c r="D11" s="16">
+        <v>0</v>
+      </c>
+      <c r="E11" s="16">
+        <v>1</v>
+      </c>
+      <c r="F11" s="16">
+        <v>1</v>
+      </c>
+      <c r="G11" s="16">
+        <v>1</v>
+      </c>
+      <c r="H11" s="16">
+        <v>1</v>
+      </c>
+      <c r="I11" s="16">
+        <v>1</v>
+      </c>
+      <c r="J11" s="16">
+        <v>1</v>
+      </c>
+      <c r="K11" s="16">
+        <v>1</v>
+      </c>
+      <c r="L11" s="16">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>1</v>
+      </c>
+      <c r="B12" s="16">
+        <v>1</v>
+      </c>
+      <c r="C12" s="16">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16">
+        <v>0</v>
+      </c>
+      <c r="E12" s="16">
+        <v>1</v>
+      </c>
+      <c r="F12" s="16">
+        <v>1</v>
+      </c>
+      <c r="G12" s="16">
+        <v>1</v>
+      </c>
+      <c r="H12" s="16">
+        <v>1</v>
+      </c>
+      <c r="I12" s="16">
+        <v>1</v>
+      </c>
+      <c r="J12" s="16">
+        <v>1</v>
+      </c>
+      <c r="K12" s="16">
+        <v>1</v>
+      </c>
+      <c r="L12" s="16">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
+        <v>1</v>
+      </c>
+      <c r="B13" s="16">
+        <v>1</v>
+      </c>
+      <c r="C13" s="16">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16">
+        <v>1</v>
+      </c>
+      <c r="E13" s="16">
+        <v>1</v>
+      </c>
+      <c r="F13" s="16">
+        <v>1</v>
+      </c>
+      <c r="G13" s="16">
+        <v>1</v>
+      </c>
+      <c r="H13" s="16">
+        <v>1</v>
+      </c>
+      <c r="I13" s="16">
+        <v>1</v>
+      </c>
+      <c r="J13" s="16">
+        <v>1</v>
+      </c>
+      <c r="K13" s="16">
+        <v>1</v>
+      </c>
+      <c r="L13" s="16">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="str">
-        <f ca="1"/>
-        <v>21-Jan</v>
-      </c>
-      <c r="B11" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="C11" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="D11" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E11" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G11" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H11" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I11" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J11" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K11" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L11" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M11" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="O11">
-        <f t="shared" ca="1" si="1"/>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <v>1</v>
+      </c>
+      <c r="B14" s="16">
+        <v>1</v>
+      </c>
+      <c r="C14" s="16">
+        <v>1</v>
+      </c>
+      <c r="D14" s="16">
+        <v>1</v>
+      </c>
+      <c r="E14" s="16">
+        <v>1</v>
+      </c>
+      <c r="F14" s="16">
+        <v>1</v>
+      </c>
+      <c r="G14" s="16">
+        <v>1</v>
+      </c>
+      <c r="H14" s="16">
+        <v>1</v>
+      </c>
+      <c r="I14" s="16">
+        <v>1</v>
+      </c>
+      <c r="J14" s="16">
+        <v>1</v>
+      </c>
+      <c r="K14" s="16">
+        <v>1</v>
+      </c>
+      <c r="L14" s="16">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="str">
-        <f ca="1"/>
-        <v>22-Jan</v>
-      </c>
-      <c r="B12" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="C12" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="D12" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E12" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G12" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H12" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I12" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J12" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K12" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L12" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M12" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="O12">
-        <f t="shared" ca="1" si="1"/>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <v>1</v>
+      </c>
+      <c r="B15" s="16">
+        <v>1</v>
+      </c>
+      <c r="C15" s="16">
+        <v>1</v>
+      </c>
+      <c r="D15" s="16">
+        <v>1</v>
+      </c>
+      <c r="E15" s="16">
+        <v>1</v>
+      </c>
+      <c r="F15" s="16">
+        <v>1</v>
+      </c>
+      <c r="G15" s="16">
+        <v>1</v>
+      </c>
+      <c r="H15" s="16">
+        <v>1</v>
+      </c>
+      <c r="I15" s="16">
+        <v>1</v>
+      </c>
+      <c r="J15" s="16">
+        <v>1</v>
+      </c>
+      <c r="K15" s="16">
+        <v>1</v>
+      </c>
+      <c r="L15" s="16">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="str">
-        <f ca="1"/>
-        <v>23-Jan</v>
-      </c>
-      <c r="B13" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="C13" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="D13" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E13" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="F13" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G13" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H13" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I13" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J13" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K13" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L13" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M13" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="O13">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="str">
-        <f ca="1"/>
-        <v>24-Jan</v>
-      </c>
-      <c r="B14" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="C14" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="D14" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E14" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="F14" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G14" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H14" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I14" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J14" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K14" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L14" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M14" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="O14">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="str">
-        <f ca="1"/>
-        <v>25-Jan</v>
-      </c>
-      <c r="B15" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="C15" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="D15" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E15" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="F15" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G15" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H15" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I15" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J15" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K15" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L15" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M15" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="O15">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
-      </c>
-    </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="str">
-        <f ca="1"/>
-        <v>26-Jan</v>
+      <c r="A16" s="16">
+        <v>1</v>
       </c>
       <c r="B16" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="C16" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="D16" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="E16" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="F16" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="G16" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="H16" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="I16" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="J16" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="K16" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="L16" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M16" s="16">
-        <f ca="1"/>
         <v>0</v>
       </c>
       <c r="N16">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="O16">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="str">
-        <f ca="1"/>
-        <v>27-Jan</v>
+      <c r="A17" s="16">
+        <v>1</v>
       </c>
       <c r="B17" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="C17" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="D17" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="E17" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="F17" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="G17" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="H17" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="I17" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="J17" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="K17" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="L17" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M17" s="16">
-        <f ca="1"/>
         <v>0</v>
       </c>
       <c r="N17">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="O17">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="str">
-        <f ca="1"/>
-        <v>28-Jan</v>
+      <c r="A18" s="16">
+        <v>1</v>
       </c>
       <c r="B18" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="C18" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="D18" s="16">
-        <f ca="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="16">
-        <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="G18" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="H18" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="I18" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="J18" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="K18" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="L18" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M18" s="16">
-        <f ca="1"/>
         <v>0</v>
       </c>
       <c r="N18">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="O18">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
+        <v>1</v>
+      </c>
+      <c r="B19" s="16">
+        <v>1</v>
+      </c>
+      <c r="C19" s="16">
+        <v>1</v>
+      </c>
+      <c r="D19" s="16">
+        <v>0</v>
+      </c>
+      <c r="E19" s="16">
+        <v>1</v>
+      </c>
+      <c r="F19" s="16">
+        <v>1</v>
+      </c>
+      <c r="G19" s="16">
+        <v>1</v>
+      </c>
+      <c r="H19" s="16">
+        <v>1</v>
+      </c>
+      <c r="I19" s="16">
+        <v>1</v>
+      </c>
+      <c r="J19" s="16">
+        <v>1</v>
+      </c>
+      <c r="K19" s="16">
+        <v>1</v>
+      </c>
+      <c r="L19" s="16">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <v>1</v>
+      </c>
+      <c r="B20" s="16">
+        <v>1</v>
+      </c>
+      <c r="C20" s="16">
+        <v>1</v>
+      </c>
+      <c r="D20" s="16">
+        <v>0</v>
+      </c>
+      <c r="E20" s="16">
+        <v>1</v>
+      </c>
+      <c r="F20" s="16">
+        <v>1</v>
+      </c>
+      <c r="G20" s="16">
+        <v>1</v>
+      </c>
+      <c r="H20" s="16">
+        <v>1</v>
+      </c>
+      <c r="I20" s="16">
+        <v>1</v>
+      </c>
+      <c r="J20" s="16">
+        <v>1</v>
+      </c>
+      <c r="K20" s="16">
+        <v>1</v>
+      </c>
+      <c r="L20" s="16">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
+        <v>1</v>
+      </c>
+      <c r="B21" s="16">
+        <v>0</v>
+      </c>
+      <c r="C21" s="16">
+        <v>1</v>
+      </c>
+      <c r="D21" s="16">
+        <v>1</v>
+      </c>
+      <c r="E21" s="16">
+        <v>1</v>
+      </c>
+      <c r="F21" s="16">
+        <v>1</v>
+      </c>
+      <c r="G21" s="16">
+        <v>1</v>
+      </c>
+      <c r="H21" s="16">
+        <v>1</v>
+      </c>
+      <c r="I21" s="16">
+        <v>1</v>
+      </c>
+      <c r="J21" s="16">
+        <v>1</v>
+      </c>
+      <c r="K21" s="16">
+        <v>1</v>
+      </c>
+      <c r="L21" s="16">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
+        <v>1</v>
+      </c>
+      <c r="B22" s="16">
+        <v>0</v>
+      </c>
+      <c r="C22" s="16">
+        <v>1</v>
+      </c>
+      <c r="D22" s="16">
+        <v>1</v>
+      </c>
+      <c r="E22" s="16">
+        <v>1</v>
+      </c>
+      <c r="F22" s="16">
+        <v>1</v>
+      </c>
+      <c r="G22" s="16">
+        <v>1</v>
+      </c>
+      <c r="H22" s="16">
+        <v>1</v>
+      </c>
+      <c r="I22" s="16">
+        <v>1</v>
+      </c>
+      <c r="J22" s="16">
+        <v>1</v>
+      </c>
+      <c r="K22" s="16">
+        <v>1</v>
+      </c>
+      <c r="L22" s="16">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
+        <v>1</v>
+      </c>
+      <c r="B23" s="16">
+        <v>0</v>
+      </c>
+      <c r="C23" s="16">
+        <v>1</v>
+      </c>
+      <c r="D23" s="16">
+        <v>1</v>
+      </c>
+      <c r="E23" s="16">
+        <v>1</v>
+      </c>
+      <c r="F23" s="16">
+        <v>1</v>
+      </c>
+      <c r="G23" s="16">
+        <v>1</v>
+      </c>
+      <c r="H23" s="16">
+        <v>1</v>
+      </c>
+      <c r="I23" s="16">
+        <v>1</v>
+      </c>
+      <c r="J23" s="16">
+        <v>1</v>
+      </c>
+      <c r="K23" s="16">
+        <v>1</v>
+      </c>
+      <c r="L23" s="16">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="16">
+        <v>1</v>
+      </c>
+      <c r="B24" s="16">
+        <v>0</v>
+      </c>
+      <c r="C24" s="16">
+        <v>1</v>
+      </c>
+      <c r="D24" s="16">
+        <v>0</v>
+      </c>
+      <c r="E24" s="16">
+        <v>1</v>
+      </c>
+      <c r="F24" s="16">
+        <v>1</v>
+      </c>
+      <c r="G24" s="16">
+        <v>1</v>
+      </c>
+      <c r="H24" s="16">
+        <v>1</v>
+      </c>
+      <c r="I24" s="16">
+        <v>1</v>
+      </c>
+      <c r="J24" s="16">
+        <v>1</v>
+      </c>
+      <c r="K24" s="16">
+        <v>1</v>
+      </c>
+      <c r="L24" s="16">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
+        <v>1</v>
+      </c>
+      <c r="B25" s="16">
+        <v>0</v>
+      </c>
+      <c r="C25" s="16">
+        <v>1</v>
+      </c>
+      <c r="D25" s="16">
+        <v>0</v>
+      </c>
+      <c r="E25" s="16">
+        <v>1</v>
+      </c>
+      <c r="F25" s="16">
+        <v>1</v>
+      </c>
+      <c r="G25" s="16">
+        <v>1</v>
+      </c>
+      <c r="H25" s="16">
+        <v>1</v>
+      </c>
+      <c r="I25" s="16">
+        <v>1</v>
+      </c>
+      <c r="J25" s="16">
+        <v>1</v>
+      </c>
+      <c r="K25" s="16">
+        <v>1</v>
+      </c>
+      <c r="L25" s="16">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="16">
+        <v>1</v>
+      </c>
+      <c r="B26" s="16">
+        <v>0</v>
+      </c>
+      <c r="C26" s="16">
+        <v>1</v>
+      </c>
+      <c r="D26" s="16">
+        <v>0</v>
+      </c>
+      <c r="E26" s="16">
+        <v>1</v>
+      </c>
+      <c r="F26" s="16">
+        <v>1</v>
+      </c>
+      <c r="G26" s="16">
+        <v>1</v>
+      </c>
+      <c r="H26" s="16">
+        <v>1</v>
+      </c>
+      <c r="I26" s="16">
+        <v>1</v>
+      </c>
+      <c r="J26" s="16">
+        <v>1</v>
+      </c>
+      <c r="K26" s="16">
+        <v>1</v>
+      </c>
+      <c r="L26" s="16">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="16">
+        <v>0</v>
+      </c>
+      <c r="B27" s="16">
+        <v>0</v>
+      </c>
+      <c r="C27" s="16">
+        <v>1</v>
+      </c>
+      <c r="D27" s="16">
+        <v>0</v>
+      </c>
+      <c r="E27" s="16">
+        <v>1</v>
+      </c>
+      <c r="F27" s="16">
+        <v>1</v>
+      </c>
+      <c r="G27" s="16">
+        <v>1</v>
+      </c>
+      <c r="H27" s="16">
+        <v>1</v>
+      </c>
+      <c r="I27" s="16">
+        <v>1</v>
+      </c>
+      <c r="J27" s="16">
+        <v>1</v>
+      </c>
+      <c r="K27" s="16">
+        <v>1</v>
+      </c>
+      <c r="L27" s="16">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="16">
+        <v>0</v>
+      </c>
+      <c r="B28" s="16">
+        <v>0</v>
+      </c>
+      <c r="C28" s="16">
+        <v>1</v>
+      </c>
+      <c r="D28" s="16">
+        <v>0</v>
+      </c>
+      <c r="E28" s="16">
+        <v>1</v>
+      </c>
+      <c r="F28" s="16">
+        <v>1</v>
+      </c>
+      <c r="G28" s="16">
+        <v>1</v>
+      </c>
+      <c r="H28" s="16">
+        <v>1</v>
+      </c>
+      <c r="I28" s="16">
+        <v>1</v>
+      </c>
+      <c r="J28" s="16">
+        <v>1</v>
+      </c>
+      <c r="K28" s="16">
+        <v>1</v>
+      </c>
+      <c r="L28" s="16">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="16">
+        <v>0</v>
+      </c>
+      <c r="B29" s="16">
+        <v>0</v>
+      </c>
+      <c r="C29" s="16">
+        <v>1</v>
+      </c>
+      <c r="D29" s="16">
+        <v>1</v>
+      </c>
+      <c r="E29" s="16">
+        <v>1</v>
+      </c>
+      <c r="F29" s="16">
+        <v>1</v>
+      </c>
+      <c r="G29" s="16">
+        <v>1</v>
+      </c>
+      <c r="H29" s="16">
+        <v>1</v>
+      </c>
+      <c r="I29" s="16">
+        <v>1</v>
+      </c>
+      <c r="J29" s="16">
+        <v>1</v>
+      </c>
+      <c r="K29" s="16">
+        <v>1</v>
+      </c>
+      <c r="L29" s="16">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="16">
+        <v>0</v>
+      </c>
+      <c r="B30" s="16">
+        <v>0</v>
+      </c>
+      <c r="C30" s="16">
+        <v>1</v>
+      </c>
+      <c r="D30" s="16">
+        <v>0</v>
+      </c>
+      <c r="E30" s="16">
+        <v>1</v>
+      </c>
+      <c r="F30" s="16">
+        <v>1</v>
+      </c>
+      <c r="G30" s="16">
+        <v>1</v>
+      </c>
+      <c r="H30" s="16">
+        <v>1</v>
+      </c>
+      <c r="I30" s="16">
+        <v>1</v>
+      </c>
+      <c r="J30" s="16">
+        <v>1</v>
+      </c>
+      <c r="K30" s="16">
+        <v>1</v>
+      </c>
+      <c r="L30" s="16">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="16">
+        <v>0</v>
+      </c>
+      <c r="B31" s="16">
+        <v>0</v>
+      </c>
+      <c r="C31" s="16">
+        <v>1</v>
+      </c>
+      <c r="D31" s="16">
+        <v>0</v>
+      </c>
+      <c r="E31" s="16">
+        <v>1</v>
+      </c>
+      <c r="F31" s="16">
+        <v>1</v>
+      </c>
+      <c r="G31" s="16">
+        <v>1</v>
+      </c>
+      <c r="H31" s="16">
+        <v>1</v>
+      </c>
+      <c r="I31" s="16">
+        <v>1</v>
+      </c>
+      <c r="J31" s="16">
+        <v>1</v>
+      </c>
+      <c r="K31" s="16">
+        <v>1</v>
+      </c>
+      <c r="L31" s="16">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="16">
+        <v>0</v>
+      </c>
+      <c r="B32" s="16">
+        <v>0</v>
+      </c>
+      <c r="C32" s="16">
+        <v>1</v>
+      </c>
+      <c r="D32" s="16">
+        <v>1</v>
+      </c>
+      <c r="E32" s="16">
+        <v>1</v>
+      </c>
+      <c r="F32" s="16">
+        <v>1</v>
+      </c>
+      <c r="G32" s="16">
+        <v>1</v>
+      </c>
+      <c r="H32" s="16">
+        <v>1</v>
+      </c>
+      <c r="I32" s="16">
+        <v>1</v>
+      </c>
+      <c r="J32" s="16">
+        <v>1</v>
+      </c>
+      <c r="K32" s="16">
+        <v>1</v>
+      </c>
+      <c r="L32" s="16">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="16">
+        <v>0</v>
+      </c>
+      <c r="B33" s="16">
+        <v>0</v>
+      </c>
+      <c r="C33" s="16">
+        <v>1</v>
+      </c>
+      <c r="D33" s="16">
+        <v>1</v>
+      </c>
+      <c r="E33" s="16">
+        <v>1</v>
+      </c>
+      <c r="F33" s="16">
+        <v>1</v>
+      </c>
+      <c r="G33" s="16">
+        <v>1</v>
+      </c>
+      <c r="H33" s="16">
+        <v>1</v>
+      </c>
+      <c r="I33" s="16">
+        <v>1</v>
+      </c>
+      <c r="J33" s="16">
+        <v>1</v>
+      </c>
+      <c r="K33" s="16">
+        <v>1</v>
+      </c>
+      <c r="L33" s="16">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="str">
-        <f ca="1"/>
-        <v>29-Jan</v>
-      </c>
-      <c r="B19" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="C19" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="D19" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E19" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G19" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H19" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I19" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J19" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K19" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L19" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M19" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="O19">
-        <f t="shared" ca="1" si="1"/>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="16">
+        <v>0</v>
+      </c>
+      <c r="B34" s="16">
+        <v>0</v>
+      </c>
+      <c r="C34" s="16">
+        <v>1</v>
+      </c>
+      <c r="D34" s="16">
+        <v>0</v>
+      </c>
+      <c r="E34" s="16">
+        <v>1</v>
+      </c>
+      <c r="F34" s="16">
+        <v>1</v>
+      </c>
+      <c r="G34" s="16">
+        <v>1</v>
+      </c>
+      <c r="H34" s="16">
+        <v>1</v>
+      </c>
+      <c r="I34" s="16">
+        <v>1</v>
+      </c>
+      <c r="J34" s="16">
+        <v>1</v>
+      </c>
+      <c r="K34" s="16">
+        <v>1</v>
+      </c>
+      <c r="L34" s="16">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="16">
+        <v>0</v>
+      </c>
+      <c r="B35" s="16">
+        <v>0</v>
+      </c>
+      <c r="C35" s="16">
+        <v>1</v>
+      </c>
+      <c r="D35" s="16">
+        <v>1</v>
+      </c>
+      <c r="E35" s="16">
+        <v>1</v>
+      </c>
+      <c r="F35" s="16">
+        <v>1</v>
+      </c>
+      <c r="G35" s="16">
+        <v>1</v>
+      </c>
+      <c r="H35" s="16">
+        <v>1</v>
+      </c>
+      <c r="I35" s="16">
+        <v>1</v>
+      </c>
+      <c r="J35" s="16">
+        <v>1</v>
+      </c>
+      <c r="K35" s="16">
+        <v>1</v>
+      </c>
+      <c r="L35" s="16">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="str">
-        <f ca="1"/>
-        <v>30-Jan</v>
-      </c>
-      <c r="B20" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="C20" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="D20" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E20" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G20" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H20" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I20" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J20" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K20" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L20" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M20" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="O20">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="str">
-        <f ca="1"/>
-        <v>31-Jan</v>
-      </c>
-      <c r="B21" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="C21" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="D21" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E21" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="F21" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G21" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H21" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I21" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J21" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K21" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L21" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M21" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="O21">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="str">
-        <f ca="1"/>
-        <v>01-Feb</v>
-      </c>
-      <c r="B22" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="C22" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="D22" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E22" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="F22" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G22" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H22" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I22" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J22" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K22" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L22" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M22" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="O22">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="str">
-        <f ca="1"/>
-        <v>02-Feb</v>
-      </c>
-      <c r="B23" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="C23" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="D23" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E23" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="F23" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G23" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H23" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I23" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J23" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K23" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L23" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M23" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="O23">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="str">
-        <f ca="1"/>
-        <v>03-Feb</v>
-      </c>
-      <c r="B24" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="C24" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="D24" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E24" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G24" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H24" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I24" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J24" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K24" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L24" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M24" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="O24">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="str">
-        <f ca="1"/>
-        <v>04-Feb</v>
-      </c>
-      <c r="B25" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="C25" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="D25" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E25" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G25" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H25" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I25" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J25" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K25" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L25" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M25" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N25">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="O25">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="str">
-        <f ca="1"/>
-        <v>05-Feb</v>
-      </c>
-      <c r="B26" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="C26" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="D26" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E26" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G26" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H26" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I26" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J26" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K26" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L26" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M26" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="O26">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="str">
-        <f ca="1"/>
-        <v>06-Feb</v>
-      </c>
-      <c r="B27" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="C27" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="D27" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E27" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G27" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H27" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I27" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J27" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K27" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L27" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M27" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="O27">
-        <f t="shared" ca="1" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="str">
-        <f ca="1"/>
-        <v>07-Feb</v>
-      </c>
-      <c r="B28" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="C28" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="D28" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E28" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G28" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H28" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I28" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J28" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K28" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L28" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M28" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N28">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="O28">
-        <f t="shared" ca="1" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="str">
-        <f ca="1"/>
-        <v>08-Feb</v>
-      </c>
-      <c r="B29" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="C29" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="D29" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E29" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="F29" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G29" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H29" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I29" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J29" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K29" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L29" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M29" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N29">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="O29">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="str">
-        <f ca="1"/>
-        <v>09-Feb</v>
-      </c>
-      <c r="B30" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="C30" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="D30" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E30" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G30" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H30" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I30" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J30" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K30" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L30" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M30" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N30">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="O30">
-        <f t="shared" ca="1" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="str">
-        <f ca="1"/>
-        <v>10-Feb</v>
-      </c>
-      <c r="B31" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="C31" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="D31" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E31" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G31" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H31" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I31" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J31" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K31" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L31" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M31" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N31">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="O31">
-        <f t="shared" ca="1" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="str">
-        <f ca="1"/>
-        <v>11-Feb</v>
-      </c>
-      <c r="B32" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="C32" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="D32" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E32" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="F32" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G32" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H32" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I32" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J32" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K32" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L32" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M32" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N32">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="O32">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="str">
-        <f ca="1"/>
-        <v>12-Feb</v>
-      </c>
-      <c r="B33" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="C33" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="D33" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E33" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="F33" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G33" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H33" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I33" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J33" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K33" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L33" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M33" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="N33">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="O33">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="str">
-        <f ca="1"/>
-        <v>13-Feb</v>
-      </c>
-      <c r="B34" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="C34" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="D34" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E34" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G34" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H34" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I34" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J34" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K34" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L34" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M34" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="N34">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="O34">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="str">
-        <f ca="1"/>
-        <v>14-Feb</v>
-      </c>
-      <c r="B35" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="C35" s="16">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="D35" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="E35" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="F35" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G35" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="H35" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I35" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J35" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K35" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="L35" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M35" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="N35">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="O35">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="str">
-        <f ca="1"/>
-        <v>15-Feb</v>
+      <c r="A36" s="16">
+        <v>0</v>
       </c>
       <c r="B36" s="16">
-        <f ca="1"/>
         <v>0</v>
       </c>
       <c r="C36" s="16">
-        <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="E36" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="F36" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="G36" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="H36" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="I36" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="J36" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="K36" s="16">
-        <f ca="1"/>
         <v>1</v>
       </c>
       <c r="L36" s="16">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="M36" s="16">
-        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="16">
+        <v>0</v>
+      </c>
+      <c r="B37" s="16">
+        <v>0</v>
+      </c>
+      <c r="C37" s="16">
+        <v>0</v>
+      </c>
+      <c r="D37" s="16">
+        <v>0</v>
+      </c>
+      <c r="E37" s="16">
+        <v>0</v>
+      </c>
+      <c r="F37" s="16">
+        <v>0</v>
+      </c>
+      <c r="G37" s="16">
+        <v>0</v>
+      </c>
+      <c r="H37" s="16">
+        <v>0</v>
+      </c>
+      <c r="I37" s="16">
+        <v>0</v>
+      </c>
+      <c r="J37" s="16">
+        <v>0</v>
+      </c>
+      <c r="K37" s="16">
+        <v>1</v>
+      </c>
+      <c r="L37" s="16">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:M35">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(A2)-ROW($A$1),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Working a bit on formatting
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36324FC6-E676-48B2-9DC6-082D983337F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876F8FA3-FA6C-4BF1-B731-F626EAB6C7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <definedName name="Banded">_xlfn.DROP(_xlfn._TRO_ALL(Report!$B:$N),1)</definedName>
     <definedName name="Banded2">_xlfn.DROP(_xlfn._TRO_ALL(Report!$R:$AD),1)</definedName>
     <definedName name="data">_xlfn.DROP(Banded,11,1)</definedName>
+    <definedName name="Dynamic">_xlfn.VSTACK(Report!$R$9:$AD$9,Banded2)</definedName>
     <definedName name="fmt" localSheetId="0">_xlfn.DROP(_xlfn._TRO_ALL(Report!$C:$N),12)</definedName>
     <definedName name="fmt" localSheetId="1">_xlfn._TRO_ALL(Summary!$A:$M)</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
@@ -646,7 +647,21 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -893,27 +908,27 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Standard Pivot Table" table="0" count="12" xr9:uid="{94886349-6B4A-4300-89B0-9F83C8B5183A}">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="totalRow" dxfId="18"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="17"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="16"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="15"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="14"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="13"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="12"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="11"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="10"/>
-      <tableStyleElement type="pageFieldValues" dxfId="9"/>
+      <tableStyleElement type="wholeTable" dxfId="22"/>
+      <tableStyleElement type="headerRow" dxfId="21"/>
+      <tableStyleElement type="totalRow" dxfId="20"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="19"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="18"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="17"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="16"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="14"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="13"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="12"/>
+      <tableStyleElement type="pageFieldValues" dxfId="11"/>
     </tableStyle>
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="8"/>
-      <tableStyleElement type="headerRow" dxfId="7"/>
-      <tableStyleElement type="totalRow" dxfId="6"/>
-      <tableStyleElement type="firstColumn" dxfId="5"/>
-      <tableStyleElement type="lastColumn" dxfId="4"/>
-      <tableStyleElement type="firstRowStripe" dxfId="3"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="2"/>
+      <tableStyleElement type="wholeTable" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="totalRow" dxfId="8"/>
+      <tableStyleElement type="firstColumn" dxfId="7"/>
+      <tableStyleElement type="lastColumn" dxfId="6"/>
+      <tableStyleElement type="firstRowStripe" dxfId="5"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -937,6 +952,77 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>17</xdr:col>
+          <xdr:colOff>7620</xdr:colOff>
+          <xdr:row>49</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>30</xdr:col>
+          <xdr:colOff>15240</xdr:colOff>
+          <xdr:row>64</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Picture 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07C580AA-3614-ECFD-1AC8-7A7A416D4E34}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="$R$9:$AD$15" spid="_x0000_s2055"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="5798820" y="9311640"/>
+              <a:ext cx="4061460" cy="2545080"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1259,16 +1345,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB114D2F-F620-446A-92CE-0CB3C9FD0F74}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB114D2F-F620-446A-92CE-0CB3C9FD0F74}">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
   <dimension ref="A7:AG68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="S52" sqref="S52"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="AG60" sqref="AG60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1785,7 +1869,7 @@
       </c>
       <c r="U15">
         <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V15">
         <f ca="1"/>
@@ -1793,27 +1877,27 @@
       </c>
       <c r="W15">
         <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X15">
         <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y15">
         <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z15">
         <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA15">
         <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB15">
         <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC15">
         <f ca="1"/>
@@ -3697,28 +3781,28 @@
         <v>0</v>
       </c>
       <c r="E56" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" s="6">
         <v>0</v>
       </c>
       <c r="G56" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K56" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L56" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M56" s="6">
         <v>1</v>
@@ -3732,7 +3816,7 @@
       </c>
       <c r="P56">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.25">
@@ -3920,12 +4004,12 @@
     <sortCondition ref="T24:T60"/>
   </sortState>
   <conditionalFormatting sqref="B10:N56">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>MOD(ROW(B10)-ROW($R$9),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q58">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3934,8 +4018,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="R10:AD15">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD(ROW(F5)-ROW($R$9),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -5606,28 +5697,28 @@
         <v>0</v>
       </c>
       <c r="C37" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" s="16">
         <v>0</v>
       </c>
       <c r="E37" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" s="16">
         <v>1</v>
@@ -5638,7 +5729,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:M35">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>MOD(ROW(A2)-ROW($A$1),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
I have improved my formatting, but I still haven't come up with a way to deal with transient tasks.
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876F8FA3-FA6C-4BF1-B731-F626EAB6C7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2C5C38-275C-48C6-A035-6677D00A28F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -647,14 +647,7 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <fill>
         <patternFill>
@@ -908,27 +901,27 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Standard Pivot Table" table="0" count="12" xr9:uid="{94886349-6B4A-4300-89B0-9F83C8B5183A}">
-      <tableStyleElement type="wholeTable" dxfId="22"/>
-      <tableStyleElement type="headerRow" dxfId="21"/>
-      <tableStyleElement type="totalRow" dxfId="20"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="19"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="18"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="17"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="16"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="15"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="14"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="13"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="12"/>
-      <tableStyleElement type="pageFieldValues" dxfId="11"/>
+      <tableStyleElement type="wholeTable" dxfId="21"/>
+      <tableStyleElement type="headerRow" dxfId="20"/>
+      <tableStyleElement type="totalRow" dxfId="19"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="18"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="17"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="16"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="15"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="14"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="13"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="12"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="11"/>
+      <tableStyleElement type="pageFieldValues" dxfId="10"/>
     </tableStyle>
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="10"/>
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="totalRow" dxfId="8"/>
-      <tableStyleElement type="firstColumn" dxfId="7"/>
-      <tableStyleElement type="lastColumn" dxfId="6"/>
-      <tableStyleElement type="firstRowStripe" dxfId="5"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="4"/>
+      <tableStyleElement type="wholeTable" dxfId="9"/>
+      <tableStyleElement type="headerRow" dxfId="8"/>
+      <tableStyleElement type="totalRow" dxfId="7"/>
+      <tableStyleElement type="firstColumn" dxfId="6"/>
+      <tableStyleElement type="lastColumn" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -981,7 +974,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$R$9:$AD$15" spid="_x0000_s2055"/>
+                  <a14:cameraTool cellRange="$R$9:$AD$15" spid="_x0000_s2056"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1351,8 +1344,8 @@
   </sheetPr>
   <dimension ref="A7:AG68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="AG60" sqref="AG60"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="R42" sqref="R42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1873,7 +1866,7 @@
       </c>
       <c r="V15">
         <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W15">
         <f ca="1"/>
@@ -3784,7 +3777,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56" s="6">
         <v>1</v>
@@ -3816,7 +3809,7 @@
       </c>
       <c r="P56">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.25">
@@ -4004,7 +3997,7 @@
     <sortCondition ref="T24:T60"/>
   </sortState>
   <conditionalFormatting sqref="B10:N56">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>MOD(ROW(B10)-ROW($R$9),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4019,7 +4012,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10:AD15">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(F5)-ROW($R$9),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5700,7 +5693,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" s="16">
         <v>1</v>
@@ -5729,7 +5722,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:M35">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(A2)-ROW($A$1),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Needed to include Bayesian work
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E856584C-924C-4A3C-AE1A-3D5C644D7245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C71CDC-07C6-4361-A56E-67EAF794678D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38340" yWindow="140" windowWidth="16440" windowHeight="15410" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-22200" yWindow="3220" windowWidth="16440" windowHeight="15410" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <definedName name="fmt" localSheetId="0">_xlfn.DROP(_xlfn._TRO_ALL(Report!$C:$K),12)</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
     <definedName name="ix">_xlfn.DROP(_xlfn._TRO_ALL(Report!$L:$L),0)</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">_xlfn.DROP(_xlfn.TRIMRANGE(LongTermTraining!$D:$O),1)</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">_xlfn.DROP(_xlfn.TRIMRANGE(LongTermTraining!$D:$P),1)</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">_xlfn.DROP(_xlfn._TRO_ALL(Report!$B:$K),1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Day</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>Power Automate Project</t>
+  </si>
+  <si>
+    <t>Bayesian Text</t>
   </si>
 </sst>
 </file>
@@ -896,7 +899,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$O$9:$X$18" spid="_x0000_s2228"/>
+                  <a14:cameraTool cellRange="$O$9:$X$18" spid="_x0000_s2229"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1159,8 +1162,8 @@
   </sheetPr>
   <dimension ref="A7:AA99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="bottomLeft" activeCell="X80" sqref="X80"/>
     </sheetView>
@@ -3131,7 +3134,7 @@
         <v>7</v>
       </c>
       <c r="M53">
-        <f t="shared" ref="M53:M77" si="1">SUM(C53:K53)</f>
+        <f t="shared" ref="M53:M76" si="1">SUM(C53:K53)</f>
         <v>8</v>
       </c>
     </row>
@@ -4411,19 +4414,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7275F8F4-F02E-491D-8929-12439DC1AD26}">
-  <dimension ref="D7:W76"/>
+  <dimension ref="D7:X76"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="18" width="3.33203125" customWidth="1"/>
+    <col min="5" max="19" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:23" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="4:23" ht="131.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:24" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="4:24" ht="131.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>0</v>
       </c>
@@ -4452,16 +4455,19 @@
         <v>19</v>
       </c>
       <c r="M8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="18" t="s">
+      <c r="P8" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="4:23" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:24" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D9" t="str" cm="1">
         <f t="array" aca="1" ref="D9:D76" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
         <v>01-Jan</v>
@@ -4499,12 +4505,15 @@
       <c r="O9">
         <v>0</v>
       </c>
-      <c r="Q9" cm="1">
-        <f t="array" ref="Q9:Q76">_xlfn.BYROW(_xlfn.DROP(_xlnm.Print_Area,,1),_xleta.SUM)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="R9" cm="1">
+        <f t="array" ref="R9:R76">_xlfn.BYROW(_xlfn.DROP(_xlnm.Print_Area,,1),_xleta.SUM)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D10" t="str">
         <f ca="1"/>
         <v>02-Jan</v>
@@ -4542,11 +4551,14 @@
       <c r="O10">
         <v>0</v>
       </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D11" t="str">
         <f ca="1"/>
         <v>03-Jan</v>
@@ -4584,14 +4596,17 @@
       <c r="O11">
         <v>0</v>
       </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D12" t="str">
         <f ca="1"/>
         <v>04-Jan</v>
@@ -4629,11 +4644,14 @@
       <c r="O12">
         <v>0</v>
       </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D13" t="str">
         <f ca="1"/>
         <v>05-Jan</v>
@@ -4671,11 +4689,14 @@
       <c r="O13">
         <v>0</v>
       </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D14" t="str">
         <f ca="1"/>
         <v>06-Jan</v>
@@ -4713,11 +4734,14 @@
       <c r="O14">
         <v>0</v>
       </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D15" t="str">
         <f ca="1"/>
         <v>07-Jan</v>
@@ -4755,11 +4779,14 @@
       <c r="O15">
         <v>0</v>
       </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D16" t="str">
         <f ca="1"/>
         <v>08-Jan</v>
@@ -4797,11 +4824,14 @@
       <c r="O16">
         <v>0</v>
       </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D17" t="str">
         <f ca="1"/>
         <v>09-Jan</v>
@@ -4839,11 +4869,14 @@
       <c r="O17">
         <v>0</v>
       </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D18" t="str">
         <f ca="1"/>
         <v>10-Jan</v>
@@ -4881,11 +4914,14 @@
       <c r="O18">
         <v>0</v>
       </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D19" t="str">
         <f ca="1"/>
         <v>11-Jan</v>
@@ -4923,11 +4959,14 @@
       <c r="O19">
         <v>0</v>
       </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D20" t="str">
         <f ca="1"/>
         <v>12-Jan</v>
@@ -4965,11 +5004,14 @@
       <c r="O20">
         <v>0</v>
       </c>
-      <c r="Q20">
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="R20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D21" t="str">
         <f ca="1"/>
         <v>13-Jan</v>
@@ -5007,11 +5049,14 @@
       <c r="O21">
         <v>0</v>
       </c>
-      <c r="Q21">
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="R21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D22" t="str">
         <f ca="1"/>
         <v>14-Jan</v>
@@ -5049,11 +5094,14 @@
       <c r="O22">
         <v>0</v>
       </c>
-      <c r="Q22">
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="R22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D23" t="str">
         <f ca="1"/>
         <v>15-Jan</v>
@@ -5091,11 +5139,14 @@
       <c r="O23">
         <v>0</v>
       </c>
-      <c r="Q23">
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="R23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D24" t="str">
         <f ca="1"/>
         <v>16-Jan</v>
@@ -5133,11 +5184,14 @@
       <c r="O24">
         <v>0</v>
       </c>
-      <c r="Q24">
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="R24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D25" t="str">
         <f ca="1"/>
         <v>17-Jan</v>
@@ -5175,11 +5229,14 @@
       <c r="O25">
         <v>0</v>
       </c>
-      <c r="Q25">
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="R25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D26" t="str">
         <f ca="1"/>
         <v>18-Jan</v>
@@ -5217,11 +5274,14 @@
       <c r="O26">
         <v>0</v>
       </c>
-      <c r="Q26">
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="R26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D27" t="str">
         <f ca="1"/>
         <v>19-Jan</v>
@@ -5259,11 +5319,14 @@
       <c r="O27">
         <v>0</v>
       </c>
-      <c r="Q27">
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="R27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D28" t="str">
         <f ca="1"/>
         <v>20-Jan</v>
@@ -5301,11 +5364,14 @@
       <c r="O28">
         <v>0</v>
       </c>
-      <c r="Q28">
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="R28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D29" t="str">
         <f ca="1"/>
         <v>21-Jan</v>
@@ -5343,11 +5409,14 @@
       <c r="O29">
         <v>0</v>
       </c>
-      <c r="Q29">
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="R29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D30" t="str">
         <f ca="1"/>
         <v>22-Jan</v>
@@ -5385,11 +5454,14 @@
       <c r="O30">
         <v>0</v>
       </c>
-      <c r="Q30">
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="R30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D31" t="str">
         <f ca="1"/>
         <v>23-Jan</v>
@@ -5427,11 +5499,14 @@
       <c r="O31">
         <v>0</v>
       </c>
-      <c r="Q31">
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="R31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D32" t="str">
         <f ca="1"/>
         <v>24-Jan</v>
@@ -5469,11 +5544,14 @@
       <c r="O32">
         <v>0</v>
       </c>
-      <c r="Q32">
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="R32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D33" t="str">
         <f ca="1"/>
         <v>25-Jan</v>
@@ -5511,11 +5589,14 @@
       <c r="O33">
         <v>0</v>
       </c>
-      <c r="Q33">
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="R33">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D34" t="str">
         <f ca="1"/>
         <v>26-Jan</v>
@@ -5553,11 +5634,14 @@
       <c r="O34">
         <v>0</v>
       </c>
-      <c r="Q34">
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="R34">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D35" t="str">
         <f ca="1"/>
         <v>27-Jan</v>
@@ -5595,11 +5679,14 @@
       <c r="O35">
         <v>0</v>
       </c>
-      <c r="Q35">
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="R35">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D36" t="str">
         <f ca="1"/>
         <v>28-Jan</v>
@@ -5637,11 +5724,14 @@
       <c r="O36">
         <v>0</v>
       </c>
-      <c r="Q36">
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="R36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D37" t="str">
         <f ca="1"/>
         <v>29-Jan</v>
@@ -5679,11 +5769,14 @@
       <c r="O37">
         <v>0</v>
       </c>
-      <c r="Q37">
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="R37">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D38" t="str">
         <f ca="1"/>
         <v>30-Jan</v>
@@ -5721,11 +5814,14 @@
       <c r="O38">
         <v>0</v>
       </c>
-      <c r="Q38">
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="R38">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D39" t="str">
         <f ca="1"/>
         <v>31-Jan</v>
@@ -5763,11 +5859,14 @@
       <c r="O39">
         <v>0</v>
       </c>
-      <c r="Q39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D40" t="str">
         <f ca="1"/>
         <v>01-Feb</v>
@@ -5805,11 +5904,14 @@
       <c r="O40">
         <v>0</v>
       </c>
-      <c r="Q40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D41" t="str">
         <f ca="1"/>
         <v>02-Feb</v>
@@ -5847,11 +5949,14 @@
       <c r="O41">
         <v>0</v>
       </c>
-      <c r="Q41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D42" t="str">
         <f ca="1"/>
         <v>03-Feb</v>
@@ -5889,11 +5994,14 @@
       <c r="O42">
         <v>0</v>
       </c>
-      <c r="Q42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="R42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D43" t="str">
         <f ca="1"/>
         <v>04-Feb</v>
@@ -5931,11 +6039,14 @@
       <c r="O43">
         <v>0</v>
       </c>
-      <c r="Q43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D44" t="str">
         <f ca="1"/>
         <v>05-Feb</v>
@@ -5973,11 +6084,14 @@
       <c r="O44">
         <v>0</v>
       </c>
-      <c r="Q44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D45" t="str">
         <f ca="1"/>
         <v>06-Feb</v>
@@ -6015,11 +6129,14 @@
       <c r="O45">
         <v>0</v>
       </c>
-      <c r="Q45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D46" t="str">
         <f ca="1"/>
         <v>07-Feb</v>
@@ -6057,11 +6174,14 @@
       <c r="O46">
         <v>0</v>
       </c>
-      <c r="Q46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D47" t="str">
         <f ca="1"/>
         <v>08-Feb</v>
@@ -6099,11 +6219,14 @@
       <c r="O47">
         <v>0</v>
       </c>
-      <c r="Q47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D48" t="str">
         <f ca="1"/>
         <v>09-Feb</v>
@@ -6141,11 +6264,14 @@
       <c r="O48">
         <v>0</v>
       </c>
-      <c r="Q48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P48">
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D49" t="str">
         <f ca="1"/>
         <v>10-Feb</v>
@@ -6183,11 +6309,14 @@
       <c r="O49">
         <v>0</v>
       </c>
-      <c r="Q49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D50" t="str">
         <f ca="1"/>
         <v>11-Feb</v>
@@ -6225,11 +6354,14 @@
       <c r="O50">
         <v>0</v>
       </c>
-      <c r="Q50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="R50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D51" t="str">
         <f ca="1"/>
         <v>12-Feb</v>
@@ -6267,11 +6399,14 @@
       <c r="O51">
         <v>0</v>
       </c>
-      <c r="Q51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="R51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D52" t="str">
         <f ca="1"/>
         <v>13-Feb</v>
@@ -6309,11 +6444,14 @@
       <c r="O52">
         <v>0</v>
       </c>
-      <c r="Q52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P52">
+        <v>0</v>
+      </c>
+      <c r="R52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D53" t="str">
         <f ca="1"/>
         <v>14-Feb</v>
@@ -6351,11 +6489,14 @@
       <c r="O53">
         <v>0</v>
       </c>
-      <c r="Q53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D54" t="str">
         <f ca="1"/>
         <v>15-Feb</v>
@@ -6393,11 +6534,14 @@
       <c r="O54">
         <v>0</v>
       </c>
-      <c r="Q54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D55" t="str">
         <f ca="1"/>
         <v>16-Feb</v>
@@ -6435,11 +6579,14 @@
       <c r="O55">
         <v>0</v>
       </c>
-      <c r="Q55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P55">
+        <v>0</v>
+      </c>
+      <c r="R55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D56" t="str">
         <f ca="1"/>
         <v>17-Feb</v>
@@ -6477,11 +6624,14 @@
       <c r="O56">
         <v>0</v>
       </c>
-      <c r="Q56">
+      <c r="P56">
+        <v>0</v>
+      </c>
+      <c r="R56">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D57" t="str">
         <f ca="1"/>
         <v>18-Feb</v>
@@ -6519,11 +6669,14 @@
       <c r="O57">
         <v>0</v>
       </c>
-      <c r="Q57">
+      <c r="P57">
+        <v>0</v>
+      </c>
+      <c r="R57">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D58" t="str">
         <f ca="1"/>
         <v>19-Feb</v>
@@ -6561,11 +6714,14 @@
       <c r="O58">
         <v>0</v>
       </c>
-      <c r="Q58">
+      <c r="P58">
+        <v>0</v>
+      </c>
+      <c r="R58">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D59" t="str">
         <f ca="1"/>
         <v>20-Feb</v>
@@ -6603,11 +6759,14 @@
       <c r="O59">
         <v>0</v>
       </c>
-      <c r="Q59">
+      <c r="P59">
+        <v>0</v>
+      </c>
+      <c r="R59">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D60" t="str">
         <f ca="1"/>
         <v>21-Feb</v>
@@ -6645,11 +6804,14 @@
       <c r="O60">
         <v>0</v>
       </c>
-      <c r="Q60">
+      <c r="P60">
+        <v>0</v>
+      </c>
+      <c r="R60">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D61" t="str">
         <f ca="1"/>
         <v>22-Feb</v>
@@ -6687,11 +6849,14 @@
       <c r="O61">
         <v>0</v>
       </c>
-      <c r="Q61">
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="R61">
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D62" t="str">
         <f ca="1"/>
         <v>23-Feb</v>
@@ -6729,11 +6894,14 @@
       <c r="O62">
         <v>0</v>
       </c>
-      <c r="Q62">
+      <c r="P62">
+        <v>0</v>
+      </c>
+      <c r="R62">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D63" t="str">
         <f ca="1"/>
         <v>24-Feb</v>
@@ -6771,11 +6939,14 @@
       <c r="O63">
         <v>0</v>
       </c>
-      <c r="Q63">
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="R63">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D64" t="str">
         <f ca="1"/>
         <v>25-Feb</v>
@@ -6813,11 +6984,14 @@
       <c r="O64">
         <v>0</v>
       </c>
-      <c r="Q64">
+      <c r="P64">
+        <v>0</v>
+      </c>
+      <c r="R64">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D65" t="str">
         <f ca="1"/>
         <v>26-Feb</v>
@@ -6855,11 +7029,14 @@
       <c r="O65">
         <v>0</v>
       </c>
-      <c r="Q65">
+      <c r="P65">
+        <v>0</v>
+      </c>
+      <c r="R65">
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D66" t="str">
         <f ca="1"/>
         <v>27-Feb</v>
@@ -6897,11 +7074,14 @@
       <c r="O66">
         <v>0</v>
       </c>
-      <c r="Q66">
+      <c r="P66">
+        <v>0</v>
+      </c>
+      <c r="R66">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D67" t="str">
         <f ca="1"/>
         <v>28-Feb</v>
@@ -6939,11 +7119,14 @@
       <c r="O67">
         <v>0</v>
       </c>
-      <c r="Q67">
+      <c r="P67">
+        <v>0</v>
+      </c>
+      <c r="R67">
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D68" t="str">
         <f ca="1"/>
         <v>01-Mar</v>
@@ -6981,11 +7164,14 @@
       <c r="O68">
         <v>0</v>
       </c>
-      <c r="Q68">
+      <c r="P68">
+        <v>0</v>
+      </c>
+      <c r="R68">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D69" t="str">
         <f ca="1"/>
         <v>02-Mar</v>
@@ -7023,11 +7209,14 @@
       <c r="O69">
         <v>0</v>
       </c>
-      <c r="Q69">
+      <c r="P69">
+        <v>0</v>
+      </c>
+      <c r="R69">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D70" t="str">
         <f ca="1"/>
         <v>03-Mar</v>
@@ -7065,11 +7254,14 @@
       <c r="O70">
         <v>0</v>
       </c>
-      <c r="Q70">
+      <c r="P70">
+        <v>0</v>
+      </c>
+      <c r="R70">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D71" t="str">
         <f ca="1"/>
         <v>04-Mar</v>
@@ -7107,11 +7299,14 @@
       <c r="O71">
         <v>0</v>
       </c>
-      <c r="Q71">
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="R71">
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D72" t="str">
         <f ca="1"/>
         <v>05-Mar</v>
@@ -7149,11 +7344,14 @@
       <c r="O72">
         <v>0</v>
       </c>
-      <c r="Q72">
+      <c r="P72">
+        <v>0</v>
+      </c>
+      <c r="R72">
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D73" t="str">
         <f ca="1"/>
         <v>06-Mar</v>
@@ -7191,11 +7389,14 @@
       <c r="O73">
         <v>0</v>
       </c>
-      <c r="Q73">
+      <c r="P73">
+        <v>0</v>
+      </c>
+      <c r="R73">
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D74" t="str">
         <f ca="1"/>
         <v>07-Mar</v>
@@ -7233,11 +7434,14 @@
       <c r="O74">
         <v>0</v>
       </c>
-      <c r="Q74">
+      <c r="P74">
+        <v>0</v>
+      </c>
+      <c r="R74">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D75" t="str">
         <f ca="1"/>
         <v>08-Mar</v>
@@ -7275,11 +7479,14 @@
       <c r="O75">
         <v>0</v>
       </c>
-      <c r="Q75">
+      <c r="P75">
+        <v>0</v>
+      </c>
+      <c r="R75">
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D76" t="str">
         <f ca="1"/>
         <v>09-Mar</v>
@@ -7317,12 +7524,15 @@
       <c r="O76">
         <v>0</v>
       </c>
-      <c r="Q76">
+      <c r="P76">
+        <v>0</v>
+      </c>
+      <c r="R76">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D9:O76">
+  <conditionalFormatting sqref="D9:P76">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(D9)-ROW($D$8),2)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Started PQ Book Read
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C71CDC-07C6-4361-A56E-67EAF794678D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9F0CF8-5DB2-4886-871C-1E0A67633AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22200" yWindow="3220" windowWidth="16440" windowHeight="15410" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-18020" yWindow="2270" windowWidth="16420" windowHeight="12240" firstSheet="1" activeTab="2" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
-    <sheet name="LongTermTraining" sheetId="3" r:id="rId2"/>
+    <sheet name="PointTraining" sheetId="4" r:id="rId2"/>
+    <sheet name="LongTermTraining" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_date">_xlfn.DROP(_xlfn._TRO_ALL(Report!$B:$B),12)</definedName>
@@ -27,7 +28,7 @@
     <definedName name="fmt" localSheetId="0">_xlfn.DROP(_xlfn._TRO_ALL(Report!$C:$K),12)</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
     <definedName name="ix">_xlfn.DROP(_xlfn._TRO_ALL(Report!$L:$L),0)</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">_xlfn.DROP(_xlfn.TRIMRANGE(LongTermTraining!$D:$P),1)</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">_xlfn.DROP(_xlfn.TRIMRANGE(LongTermTraining!$D:$P),1)</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">_xlfn.DROP(_xlfn._TRO_ALL(Report!$B:$K),1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Day</t>
   </si>
@@ -154,6 +155,18 @@
   </si>
   <si>
     <t>Bayesian Text</t>
+  </si>
+  <si>
+    <t>Daily Task Count</t>
+  </si>
+  <si>
+    <t>Recipe cards from Ken Puls</t>
+  </si>
+  <si>
+    <t>Setup work on Bayesian text</t>
+  </si>
+  <si>
+    <t>PQ:25</t>
   </si>
 </sst>
 </file>
@@ -256,7 +269,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +297,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -495,7 +514,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -548,6 +567,16 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -876,15 +905,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>14</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>10160</xdr:colOff>
           <xdr:row>58</xdr:row>
-          <xdr:rowOff>82550</xdr:rowOff>
+          <xdr:rowOff>81280</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
-          <xdr:colOff>34290</xdr:colOff>
+          <xdr:colOff>3810</xdr:colOff>
           <xdr:row>76</xdr:row>
-          <xdr:rowOff>154940</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -899,7 +928,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$O$9:$X$18" spid="_x0000_s2229"/>
+                  <a14:cameraTool cellRange="$O$9:$X$18" spid="_x0000_s2243"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -913,8 +942,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="5118100" y="10763250"/>
-              <a:ext cx="3378200" cy="3048000"/>
+              <a:off x="4353560" y="10761980"/>
+              <a:ext cx="3365500" cy="3022600"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -937,7 +966,95 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5D9D0EE-AE4F-F07C-FF1E-682E12701F23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3314700" y="1059180"/>
+          <a:ext cx="175260" cy="1531620"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="vert270" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t> Week Num</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
+<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
+  <bag type="Checkbox"/>
+  <bag type="XFControls">
+    <bagId k="CellControl">0</bagId>
+  </bag>
+  <bag type="XFComplement">
+    <bagId k="XFControls">1</bagId>
+  </bag>
+  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
+    <a k="MappedFeaturePropertyBags">
+      <bagId>2</bagId>
+    </a>
+  </bag>
+</FeaturePropertyBags>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1165,7 +1282,7 @@
     <sheetView topLeftCell="A4" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="X80" sqref="X80"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1174,7 +1291,7 @@
     <col min="4" max="4" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.33203125" customWidth="1"/>
     <col min="6" max="8" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="3.33203125" customWidth="1"/>
+    <col min="9" max="13" width="3.33203125" customWidth="1"/>
     <col min="15" max="15" width="19.109375" customWidth="1"/>
     <col min="16" max="24" width="3.33203125" style="11" bestFit="1" customWidth="1"/>
   </cols>
@@ -1216,7 +1333,9 @@
         <v>7</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+      <c r="M9" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="4" t="s">
         <v>14</v>
@@ -1252,7 +1371,7 @@
     </row>
     <row r="10" spans="1:27" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="str" cm="1">
-        <f t="array" aca="1" ref="B10:B77" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
+        <f t="array" aca="1" ref="B10:B78" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
         <v>01-Jan</v>
       </c>
       <c r="C10" s="5"/>
@@ -1264,6 +1383,10 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="12"/>
+      <c r="M10" cm="1">
+        <f t="array" ref="M10:M78">_xlfn.BYROW(_xlfn.DROP(Banded,,1),_xleta.SUM)</f>
+        <v>0</v>
+      </c>
       <c r="O10" s="14" cm="1">
         <f t="array" aca="1" ref="O10:X18" ca="1">_xlfn.PIVOTBY(ix,,data,_xleta.SUM,0,0)</f>
         <v>3</v>
@@ -1319,6 +1442,9 @@
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="5"/>
+      <c r="M11">
+        <v>0</v>
+      </c>
       <c r="O11" s="14">
         <f ca="1"/>
         <v>4</v>
@@ -1377,6 +1503,9 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="5"/>
+      <c r="M12">
+        <v>0</v>
+      </c>
       <c r="O12" s="14">
         <f ca="1"/>
         <v>5</v>
@@ -1435,6 +1564,9 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="5"/>
+      <c r="M13">
+        <v>0</v>
+      </c>
       <c r="O13" s="14">
         <f ca="1"/>
         <v>6</v>
@@ -1493,6 +1625,9 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="5"/>
+      <c r="M14">
+        <v>0</v>
+      </c>
       <c r="O14" s="14">
         <f ca="1"/>
         <v>7</v>
@@ -1548,6 +1683,9 @@
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="5"/>
+      <c r="M15">
+        <v>0</v>
+      </c>
       <c r="O15" s="14">
         <f ca="1"/>
         <v>8</v>
@@ -1603,6 +1741,9 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="5"/>
+      <c r="M16">
+        <v>0</v>
+      </c>
       <c r="O16" s="14">
         <f ca="1"/>
         <v>9</v>
@@ -1657,6 +1798,9 @@
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="5"/>
+      <c r="M17">
+        <v>0</v>
+      </c>
       <c r="O17" s="14">
         <f ca="1"/>
         <v>10</v>
@@ -1712,6 +1856,9 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="5"/>
+      <c r="M18">
+        <v>0</v>
+      </c>
       <c r="O18" s="14">
         <f ca="1"/>
         <v>11</v>
@@ -1722,7 +1869,7 @@
       </c>
       <c r="Q18" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R18" s="11">
         <f ca="1"/>
@@ -1730,11 +1877,11 @@
       </c>
       <c r="S18" s="11">
         <f ca="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T18" s="11">
         <f ca="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U18" s="11">
         <f ca="1"/>
@@ -1746,11 +1893,11 @@
       </c>
       <c r="W18" s="11">
         <f ca="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X18" s="11">
         <f ca="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:24" x14ac:dyDescent="0.25">
@@ -1767,6 +1914,9 @@
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="5"/>
+      <c r="M19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="str">
@@ -1782,6 +1932,9 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="5"/>
+      <c r="M20">
+        <v>0</v>
+      </c>
       <c r="P20" s="15"/>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.25">
@@ -1817,11 +1970,10 @@
         <v>0</v>
       </c>
       <c r="L21" cm="1">
-        <f t="array" aca="1" ref="L21:L77" ca="1">WEEKNUM(_date+0)</f>
+        <f t="array" aca="1" ref="L21:L78" ca="1">WEEKNUM(_date+0)</f>
         <v>3</v>
       </c>
       <c r="M21">
-        <f t="shared" ref="M21:M52" si="0">SUM(C21:K21)</f>
         <v>6</v>
       </c>
     </row>
@@ -1862,7 +2014,6 @@
         <v>3</v>
       </c>
       <c r="M22">
-        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -1903,7 +2054,6 @@
         <v>3</v>
       </c>
       <c r="M23">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="P23" s="15"/>
@@ -1945,7 +2095,6 @@
         <v>3</v>
       </c>
       <c r="M24">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -1986,7 +2135,6 @@
         <v>3</v>
       </c>
       <c r="M25">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -2027,7 +2175,6 @@
         <v>3</v>
       </c>
       <c r="M26">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -2068,7 +2215,6 @@
         <v>3</v>
       </c>
       <c r="M27">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -2109,7 +2255,6 @@
         <v>4</v>
       </c>
       <c r="M28">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -2150,7 +2295,6 @@
         <v>4</v>
       </c>
       <c r="M29">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -2191,7 +2335,6 @@
         <v>4</v>
       </c>
       <c r="M30">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -2232,7 +2375,6 @@
         <v>4</v>
       </c>
       <c r="M31">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -2273,7 +2415,6 @@
         <v>4</v>
       </c>
       <c r="M32">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -2314,7 +2455,6 @@
         <v>4</v>
       </c>
       <c r="M33">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -2355,7 +2495,6 @@
         <v>4</v>
       </c>
       <c r="M34">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -2396,7 +2535,6 @@
         <v>5</v>
       </c>
       <c r="M35">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -2437,7 +2575,6 @@
         <v>5</v>
       </c>
       <c r="M36">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -2478,7 +2615,6 @@
         <v>5</v>
       </c>
       <c r="M37">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -2519,7 +2655,6 @@
         <v>5</v>
       </c>
       <c r="M38">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -2560,7 +2695,6 @@
         <v>5</v>
       </c>
       <c r="M39">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -2601,7 +2735,6 @@
         <v>5</v>
       </c>
       <c r="M40">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -2642,7 +2775,6 @@
         <v>5</v>
       </c>
       <c r="M41">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -2683,7 +2815,6 @@
         <v>6</v>
       </c>
       <c r="M42">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -2724,7 +2855,6 @@
         <v>6</v>
       </c>
       <c r="M43">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -2765,7 +2895,6 @@
         <v>6</v>
       </c>
       <c r="M44">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -2806,7 +2935,6 @@
         <v>6</v>
       </c>
       <c r="M45">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -2847,7 +2975,6 @@
         <v>6</v>
       </c>
       <c r="M46">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -2888,7 +3015,6 @@
         <v>6</v>
       </c>
       <c r="M47">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -2929,7 +3055,6 @@
         <v>6</v>
       </c>
       <c r="M48">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -2970,7 +3095,6 @@
         <v>7</v>
       </c>
       <c r="M49">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -3011,7 +3135,6 @@
         <v>7</v>
       </c>
       <c r="M50">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -3052,7 +3175,6 @@
         <v>7</v>
       </c>
       <c r="M51">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -3093,7 +3215,6 @@
         <v>7</v>
       </c>
       <c r="M52">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -3134,7 +3255,6 @@
         <v>7</v>
       </c>
       <c r="M53">
-        <f t="shared" ref="M53:M76" si="1">SUM(C53:K53)</f>
         <v>8</v>
       </c>
     </row>
@@ -3175,7 +3295,6 @@
         <v>7</v>
       </c>
       <c r="M54">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -3216,7 +3335,6 @@
         <v>7</v>
       </c>
       <c r="M55">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -3257,7 +3375,6 @@
         <v>8</v>
       </c>
       <c r="M56">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -3298,7 +3415,6 @@
         <v>8</v>
       </c>
       <c r="M57">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -3339,7 +3455,6 @@
         <v>8</v>
       </c>
       <c r="M58">
-        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -3380,7 +3495,6 @@
         <v>8</v>
       </c>
       <c r="M59">
-        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -3421,7 +3535,6 @@
         <v>8</v>
       </c>
       <c r="M60">
-        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -3462,7 +3575,6 @@
         <v>8</v>
       </c>
       <c r="M61">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -3503,7 +3615,6 @@
         <v>8</v>
       </c>
       <c r="M62">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -3544,7 +3655,6 @@
         <v>9</v>
       </c>
       <c r="M63">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -3585,7 +3695,6 @@
         <v>9</v>
       </c>
       <c r="M64">
-        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -3626,7 +3735,6 @@
         <v>9</v>
       </c>
       <c r="M65">
-        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -3667,7 +3775,6 @@
         <v>9</v>
       </c>
       <c r="M66">
-        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -3708,7 +3815,6 @@
         <v>9</v>
       </c>
       <c r="M67">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -3749,7 +3855,6 @@
         <v>9</v>
       </c>
       <c r="M68">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -3790,7 +3895,6 @@
         <v>9</v>
       </c>
       <c r="M69">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -3831,7 +3935,6 @@
         <v>10</v>
       </c>
       <c r="M70">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -3872,7 +3975,6 @@
         <v>10</v>
       </c>
       <c r="M71">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -3913,7 +4015,6 @@
         <v>10</v>
       </c>
       <c r="M72">
-        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -3954,7 +4055,6 @@
         <v>10</v>
       </c>
       <c r="M73">
-        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -3995,7 +4095,6 @@
         <v>10</v>
       </c>
       <c r="M74">
-        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -4036,7 +4135,6 @@
         <v>10</v>
       </c>
       <c r="M75">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -4077,7 +4175,6 @@
         <v>10</v>
       </c>
       <c r="M76">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -4090,7 +4187,7 @@
         <v>1</v>
       </c>
       <c r="D77" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" s="16">
         <v>1</v>
@@ -4118,21 +4215,48 @@
         <v>11</v>
       </c>
       <c r="M77">
-        <f>SUM(C77:K77)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B78" s="9"/>
-      <c r="C78" s="16"/>
-      <c r="D78" s="16"/>
-      <c r="E78" s="16"/>
-      <c r="F78" s="16"/>
-      <c r="G78" s="16"/>
-      <c r="H78" s="16"/>
-      <c r="I78" s="16"/>
-      <c r="J78" s="16"/>
-      <c r="K78" s="16"/>
+      <c r="B78" s="9" t="str">
+        <f ca="1"/>
+        <v>10-Mar</v>
+      </c>
+      <c r="C78" s="16">
+        <v>0</v>
+      </c>
+      <c r="D78" s="16">
+        <v>0</v>
+      </c>
+      <c r="E78" s="16">
+        <v>0</v>
+      </c>
+      <c r="F78" s="16">
+        <v>1</v>
+      </c>
+      <c r="G78" s="16">
+        <v>1</v>
+      </c>
+      <c r="H78" s="16">
+        <v>0</v>
+      </c>
+      <c r="I78" s="16">
+        <v>0</v>
+      </c>
+      <c r="J78" s="16">
+        <v>1</v>
+      </c>
+      <c r="K78" s="16">
+        <v>1</v>
+      </c>
+      <c r="L78">
+        <f ca="1"/>
+        <v>11</v>
+      </c>
+      <c r="M78">
+        <v>4</v>
+      </c>
     </row>
     <row r="79" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B79" s="9"/>
@@ -4413,11 +4537,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EF4EBB-A76D-4834-A49E-430EF56D9D9D}">
+  <dimension ref="A5:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7275F8F4-F02E-491D-8929-12439DC1AD26}">
-  <dimension ref="D7:X76"/>
+  <dimension ref="D7:X77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="V29" sqref="V29"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="T82" sqref="T82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4426,7 +4583,7 @@
   </cols>
   <sheetData>
     <row r="7" spans="4:24" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="4:24" ht="131.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:24" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>0</v>
       </c>
@@ -4469,7 +4626,7 @@
     </row>
     <row r="9" spans="4:24" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D9" t="str" cm="1">
-        <f t="array" aca="1" ref="D9:D76" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
+        <f t="array" aca="1" ref="D9:D77" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
         <v>01-Jan</v>
       </c>
       <c r="E9">
@@ -4509,7 +4666,7 @@
         <v>0</v>
       </c>
       <c r="R9" cm="1">
-        <f t="array" ref="R9:R76">_xlfn.BYROW(_xlfn.DROP(_xlnm.Print_Area,,1),_xleta.SUM)</f>
+        <f t="array" ref="R9:R77">_xlfn.BYROW(_xlfn.DROP(_xlnm.Print_Area,,1),_xleta.SUM)</f>
         <v>0</v>
       </c>
     </row>
@@ -6991,7 +7148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D65" t="str">
         <f ca="1"/>
         <v>26-Feb</v>
@@ -7036,7 +7193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D66" t="str">
         <f ca="1"/>
         <v>27-Feb</v>
@@ -7081,7 +7238,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D67" t="str">
         <f ca="1"/>
         <v>28-Feb</v>
@@ -7126,7 +7283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D68" t="str">
         <f ca="1"/>
         <v>01-Mar</v>
@@ -7171,7 +7328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D69" t="str">
         <f ca="1"/>
         <v>02-Mar</v>
@@ -7216,7 +7373,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D70" t="str">
         <f ca="1"/>
         <v>03-Mar</v>
@@ -7261,7 +7418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D71" t="str">
         <f ca="1"/>
         <v>04-Mar</v>
@@ -7306,7 +7463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D72" t="str">
         <f ca="1"/>
         <v>05-Mar</v>
@@ -7351,7 +7508,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D73" t="str">
         <f ca="1"/>
         <v>06-Mar</v>
@@ -7396,7 +7553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D74" t="str">
         <f ca="1"/>
         <v>07-Mar</v>
@@ -7441,7 +7598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D75" t="str">
         <f ca="1"/>
         <v>08-Mar</v>
@@ -7486,7 +7643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D76" t="str">
         <f ca="1"/>
         <v>09-Mar</v>
@@ -7531,8 +7688,56 @@
         <v>2</v>
       </c>
     </row>
+    <row r="77" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D77" t="str">
+        <f ca="1"/>
+        <v>10-Mar</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77">
+        <v>0</v>
+      </c>
+      <c r="O77">
+        <v>0</v>
+      </c>
+      <c r="P77">
+        <v>1</v>
+      </c>
+      <c r="R77">
+        <v>1</v>
+      </c>
+      <c r="U77" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D9:P76">
+  <conditionalFormatting sqref="D9:P76 E77">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(D9)-ROW($D$8),2)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add Power Conversion class to Long Term Training list
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2A15EF-0387-4C4A-8760-82B74C6C8FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B228F5D-BA49-40A2-B5ED-2ED08B6BBED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32760" yWindow="590" windowWidth="27450" windowHeight="12340" activeTab="2" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-32850" yWindow="2230" windowWidth="27450" windowHeight="12340" activeTab="2" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <definedName name="fmt" localSheetId="0">_xlfn.DROP(_xlfn._TRO_ALL(Report!$C:$K),12)</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
     <definedName name="ix">_xlfn.DROP(_xlfn._TRO_ALL(Report!$L:$L),0)</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">_xlfn.DROP(_xlfn.TRIMRANGE(LongTermTraining!$D:$P),1)</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">_xlfn.DROP(_xlfn.TRIMRANGE(LongTermTraining!$D:$Q),1)</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">_xlfn.DROP(_xlfn._TRO_ALL(Report!$B:$K),1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Day</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t>Setup work on Bayesian text</t>
+  </si>
+  <si>
+    <t>Writeup Chi-Square notes</t>
+  </si>
+  <si>
+    <t>CSS: Flexbox FroggyPro step 10</t>
+  </si>
+  <si>
+    <t>Power Conversion Class</t>
   </si>
 </sst>
 </file>
@@ -591,35 +600,7 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <fill>
         <patternFill>
@@ -880,27 +861,27 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Standard Pivot Table" table="0" count="12" xr9:uid="{94886349-6B4A-4300-89B0-9F83C8B5183A}">
-      <tableStyleElement type="wholeTable" dxfId="26"/>
-      <tableStyleElement type="headerRow" dxfId="25"/>
-      <tableStyleElement type="totalRow" dxfId="24"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="23"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="22"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="21"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="20"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="19"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="18"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="17"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="16"/>
-      <tableStyleElement type="pageFieldValues" dxfId="15"/>
+      <tableStyleElement type="wholeTable" dxfId="22"/>
+      <tableStyleElement type="headerRow" dxfId="21"/>
+      <tableStyleElement type="totalRow" dxfId="20"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="19"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="18"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="17"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="16"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="14"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="13"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="12"/>
+      <tableStyleElement type="pageFieldValues" dxfId="11"/>
     </tableStyle>
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="14"/>
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="totalRow" dxfId="12"/>
-      <tableStyleElement type="firstColumn" dxfId="11"/>
-      <tableStyleElement type="lastColumn" dxfId="10"/>
-      <tableStyleElement type="firstRowStripe" dxfId="9"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="8"/>
+      <tableStyleElement type="wholeTable" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="totalRow" dxfId="8"/>
+      <tableStyleElement type="firstColumn" dxfId="7"/>
+      <tableStyleElement type="lastColumn" dxfId="6"/>
+      <tableStyleElement type="firstRowStripe" dxfId="5"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -930,15 +911,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>14</xdr:col>
-          <xdr:colOff>10160</xdr:colOff>
+          <xdr:colOff>8890</xdr:colOff>
           <xdr:row>58</xdr:row>
-          <xdr:rowOff>81280</xdr:rowOff>
+          <xdr:rowOff>80010</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
-          <xdr:colOff>2540</xdr:colOff>
-          <xdr:row>76</xdr:row>
-          <xdr:rowOff>116840</xdr:rowOff>
+          <xdr:colOff>6350</xdr:colOff>
+          <xdr:row>78</xdr:row>
+          <xdr:rowOff>62230</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -953,7 +934,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$O$9:$X$18" spid="_x0000_s2253"/>
+                  <a14:cameraTool cellRange="$O$9:$X$18" spid="_x0000_s2262"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -967,8 +948,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="4353560" y="10761980"/>
-              <a:ext cx="3365500" cy="3022600"/>
+              <a:off x="4352290" y="11021060"/>
+              <a:ext cx="3365500" cy="3282950"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1027,11 +1008,7 @@
           <a:schemeClr val="lt1"/>
         </a:solidFill>
         <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -1054,7 +1031,11 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </a:rPr>
             <a:t> Week Num</a:t>
           </a:r>
         </a:p>
@@ -1305,9 +1286,9 @@
   <dimension ref="A7:AA99"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="X80" sqref="X80"/>
+      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1323,7 +1304,7 @@
   <sheetData>
     <row r="7" spans="1:27" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:27" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:27" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" ht="140.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1890,39 +1871,39 @@
       </c>
       <c r="P18" s="11">
         <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="Q18" s="11">
+        <f ca="1"/>
         <v>2</v>
       </c>
-      <c r="Q18" s="11">
-        <f ca="1"/>
-        <v>2</v>
-      </c>
       <c r="R18" s="11">
         <f ca="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S18" s="11">
         <f ca="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T18" s="11">
         <f ca="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U18" s="11">
         <f ca="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V18" s="11">
         <f ca="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W18" s="11">
         <f ca="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X18" s="11">
         <f ca="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:24" x14ac:dyDescent="0.25">
@@ -3723,7 +3704,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B65" s="9" t="str">
         <f ca="1"/>
         <v>25-Feb</v>
@@ -3763,7 +3744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B66" s="9" t="str">
         <f ca="1"/>
         <v>26-Feb</v>
@@ -3803,7 +3784,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B67" s="9" t="str">
         <f ca="1"/>
         <v>27-Feb</v>
@@ -3843,7 +3824,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B68" s="9" t="str">
         <f ca="1"/>
         <v>28-Feb</v>
@@ -3883,7 +3864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B69" s="9" t="str">
         <f ca="1"/>
         <v>01-Mar</v>
@@ -3923,7 +3904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B70" s="9" t="str">
         <f ca="1"/>
         <v>02-Mar</v>
@@ -3963,7 +3944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B71" s="9" t="str">
         <f ca="1"/>
         <v>03-Mar</v>
@@ -4003,7 +3984,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B72" s="9" t="str">
         <f ca="1"/>
         <v>04-Mar</v>
@@ -4043,7 +4024,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B73" s="9" t="str">
         <f ca="1"/>
         <v>05-Mar</v>
@@ -4083,7 +4064,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B74" s="9" t="str">
         <f ca="1"/>
         <v>06-Mar</v>
@@ -4123,7 +4104,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B75" s="9" t="str">
         <f ca="1"/>
         <v>07-Mar</v>
@@ -4163,7 +4144,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B76" s="9" t="str">
         <f ca="1"/>
         <v>08-Mar</v>
@@ -4203,7 +4184,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B77" s="9" t="str">
         <f ca="1"/>
         <v>09-Mar</v>
@@ -4243,7 +4224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B78" s="9" t="str">
         <f ca="1"/>
         <v>10-Mar</v>
@@ -4283,47 +4264,50 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B79" s="9" t="str">
         <f ca="1"/>
         <v>11-Mar</v>
       </c>
       <c r="C79" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D79" s="16">
         <v>0</v>
       </c>
       <c r="E79" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G79" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H79" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I79" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J79" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K79" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L79">
         <f ca="1"/>
         <v>11</v>
       </c>
       <c r="M79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="Z79" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B80" s="9"/>
       <c r="C80" s="16"/>
       <c r="D80" s="16"/>
@@ -4568,17 +4552,17 @@
     <sortCondition ref="Q24:Q60"/>
   </sortState>
   <conditionalFormatting sqref="B10:K79">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>MOD(ROW(XEJ10)-ROW($O$9),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:K77">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>MOD(ROW(XEM10)-ROW($O$9),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9:X18">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>MOD(ROW(O9)-ROW($O$9),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4591,10 +4575,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EF4EBB-A76D-4834-A49E-430EF56D9D9D}">
-  <dimension ref="A5:B6"/>
+  <dimension ref="A5:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4613,6 +4597,14 @@
       </c>
       <c r="B6" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -4622,22 +4614,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7275F8F4-F02E-491D-8929-12439DC1AD26}">
-  <dimension ref="D7:X78"/>
+  <dimension ref="D7:Y78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="V75" sqref="V75"/>
+      <selection pane="bottomLeft" activeCell="V68" sqref="V68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="16" width="3.33203125" style="11" customWidth="1"/>
-    <col min="17" max="19" width="3.33203125" customWidth="1"/>
+    <col min="5" max="17" width="3.33203125" style="11" customWidth="1"/>
+    <col min="18" max="20" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:24" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="4:24" ht="131.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:25" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="4:25" ht="131.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>0</v>
       </c>
@@ -4672,13 +4664,16 @@
         <v>22</v>
       </c>
       <c r="O8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P8" s="18" t="s">
+      <c r="Q8" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="4:24" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:25" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D9" t="str" cm="1">
         <f t="array" aca="1" ref="D9:D78" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
         <v>01-Jan</v>
@@ -4719,12 +4714,15 @@
       <c r="P9" s="11">
         <v>0</v>
       </c>
-      <c r="R9" cm="1">
-        <f t="array" ref="R9:R78">_xlfn.BYROW(_xlfn.DROP(_xlnm.Print_Area,,1),_xleta.SUM)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="Q9" s="11">
+        <v>0</v>
+      </c>
+      <c r="S9" cm="1">
+        <f t="array" ref="S9:S78">_xlfn.BYROW(_xlfn.DROP(_xlnm.Print_Area,,1),_xleta.SUM)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D10" t="str">
         <f ca="1"/>
         <v>02-Jan</v>
@@ -4765,11 +4763,14 @@
       <c r="P10" s="11">
         <v>0</v>
       </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="Q10" s="11">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D11" t="str">
         <f ca="1"/>
         <v>03-Jan</v>
@@ -4810,14 +4811,17 @@
       <c r="P11" s="11">
         <v>0</v>
       </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="Q11" s="11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D12" t="str">
         <f ca="1"/>
         <v>04-Jan</v>
@@ -4858,11 +4862,14 @@
       <c r="P12" s="11">
         <v>0</v>
       </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="Q12" s="11">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D13" t="str">
         <f ca="1"/>
         <v>05-Jan</v>
@@ -4903,11 +4910,14 @@
       <c r="P13" s="11">
         <v>0</v>
       </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="Q13" s="11">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D14" t="str">
         <f ca="1"/>
         <v>06-Jan</v>
@@ -4948,11 +4958,14 @@
       <c r="P14" s="11">
         <v>0</v>
       </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="Q14" s="11">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D15" t="str">
         <f ca="1"/>
         <v>07-Jan</v>
@@ -4993,11 +5006,14 @@
       <c r="P15" s="11">
         <v>0</v>
       </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="Q15" s="11">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D16" t="str">
         <f ca="1"/>
         <v>08-Jan</v>
@@ -5038,11 +5054,14 @@
       <c r="P16" s="11">
         <v>0</v>
       </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q16" s="11">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D17" t="str">
         <f ca="1"/>
         <v>09-Jan</v>
@@ -5083,11 +5102,14 @@
       <c r="P17" s="11">
         <v>0</v>
       </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q17" s="11">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D18" t="str">
         <f ca="1"/>
         <v>10-Jan</v>
@@ -5128,11 +5150,14 @@
       <c r="P18" s="11">
         <v>0</v>
       </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q18" s="11">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D19" t="str">
         <f ca="1"/>
         <v>11-Jan</v>
@@ -5173,11 +5198,14 @@
       <c r="P19" s="11">
         <v>0</v>
       </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q19" s="11">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D20" t="str">
         <f ca="1"/>
         <v>12-Jan</v>
@@ -5218,11 +5246,14 @@
       <c r="P20" s="11">
         <v>0</v>
       </c>
-      <c r="R20">
+      <c r="Q20" s="11">
+        <v>0</v>
+      </c>
+      <c r="S20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D21" t="str">
         <f ca="1"/>
         <v>13-Jan</v>
@@ -5263,11 +5294,14 @@
       <c r="P21" s="11">
         <v>0</v>
       </c>
-      <c r="R21">
+      <c r="Q21" s="11">
+        <v>0</v>
+      </c>
+      <c r="S21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D22" t="str">
         <f ca="1"/>
         <v>14-Jan</v>
@@ -5308,11 +5342,14 @@
       <c r="P22" s="11">
         <v>0</v>
       </c>
-      <c r="R22">
+      <c r="Q22" s="11">
+        <v>0</v>
+      </c>
+      <c r="S22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D23" t="str">
         <f ca="1"/>
         <v>15-Jan</v>
@@ -5353,11 +5390,14 @@
       <c r="P23" s="11">
         <v>0</v>
       </c>
-      <c r="R23">
+      <c r="Q23" s="11">
+        <v>0</v>
+      </c>
+      <c r="S23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D24" t="str">
         <f ca="1"/>
         <v>16-Jan</v>
@@ -5398,11 +5438,14 @@
       <c r="P24" s="11">
         <v>0</v>
       </c>
-      <c r="R24">
+      <c r="Q24" s="11">
+        <v>0</v>
+      </c>
+      <c r="S24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D25" t="str">
         <f ca="1"/>
         <v>17-Jan</v>
@@ -5443,11 +5486,14 @@
       <c r="P25" s="11">
         <v>0</v>
       </c>
-      <c r="R25">
+      <c r="Q25" s="11">
+        <v>0</v>
+      </c>
+      <c r="S25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D26" t="str">
         <f ca="1"/>
         <v>18-Jan</v>
@@ -5488,11 +5534,14 @@
       <c r="P26" s="11">
         <v>0</v>
       </c>
-      <c r="R26">
+      <c r="Q26" s="11">
+        <v>0</v>
+      </c>
+      <c r="S26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D27" t="str">
         <f ca="1"/>
         <v>19-Jan</v>
@@ -5533,11 +5582,14 @@
       <c r="P27" s="11">
         <v>0</v>
       </c>
-      <c r="R27">
+      <c r="Q27" s="11">
+        <v>0</v>
+      </c>
+      <c r="S27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D28" t="str">
         <f ca="1"/>
         <v>20-Jan</v>
@@ -5578,11 +5630,14 @@
       <c r="P28" s="11">
         <v>0</v>
       </c>
-      <c r="R28">
+      <c r="Q28" s="11">
+        <v>0</v>
+      </c>
+      <c r="S28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D29" t="str">
         <f ca="1"/>
         <v>21-Jan</v>
@@ -5623,11 +5678,14 @@
       <c r="P29" s="11">
         <v>0</v>
       </c>
-      <c r="R29">
+      <c r="Q29" s="11">
+        <v>0</v>
+      </c>
+      <c r="S29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D30" t="str">
         <f ca="1"/>
         <v>22-Jan</v>
@@ -5668,11 +5726,14 @@
       <c r="P30" s="11">
         <v>0</v>
       </c>
-      <c r="R30">
+      <c r="Q30" s="11">
+        <v>0</v>
+      </c>
+      <c r="S30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D31" t="str">
         <f ca="1"/>
         <v>23-Jan</v>
@@ -5713,11 +5774,14 @@
       <c r="P31" s="11">
         <v>0</v>
       </c>
-      <c r="R31">
+      <c r="Q31" s="11">
+        <v>0</v>
+      </c>
+      <c r="S31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D32" t="str">
         <f ca="1"/>
         <v>24-Jan</v>
@@ -5758,11 +5822,14 @@
       <c r="P32" s="11">
         <v>0</v>
       </c>
-      <c r="R32">
+      <c r="Q32" s="11">
+        <v>0</v>
+      </c>
+      <c r="S32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D33" t="str">
         <f ca="1"/>
         <v>25-Jan</v>
@@ -5803,11 +5870,14 @@
       <c r="P33" s="11">
         <v>0</v>
       </c>
-      <c r="R33">
+      <c r="Q33" s="11">
+        <v>0</v>
+      </c>
+      <c r="S33">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D34" t="str">
         <f ca="1"/>
         <v>26-Jan</v>
@@ -5848,11 +5918,14 @@
       <c r="P34" s="11">
         <v>0</v>
       </c>
-      <c r="R34">
+      <c r="Q34" s="11">
+        <v>0</v>
+      </c>
+      <c r="S34">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D35" t="str">
         <f ca="1"/>
         <v>27-Jan</v>
@@ -5893,11 +5966,14 @@
       <c r="P35" s="11">
         <v>0</v>
       </c>
-      <c r="R35">
+      <c r="Q35" s="11">
+        <v>0</v>
+      </c>
+      <c r="S35">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D36" t="str">
         <f ca="1"/>
         <v>28-Jan</v>
@@ -5938,11 +6014,14 @@
       <c r="P36" s="11">
         <v>0</v>
       </c>
-      <c r="R36">
+      <c r="Q36" s="11">
+        <v>0</v>
+      </c>
+      <c r="S36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D37" t="str">
         <f ca="1"/>
         <v>29-Jan</v>
@@ -5983,11 +6062,14 @@
       <c r="P37" s="11">
         <v>0</v>
       </c>
-      <c r="R37">
+      <c r="Q37" s="11">
+        <v>0</v>
+      </c>
+      <c r="S37">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D38" t="str">
         <f ca="1"/>
         <v>30-Jan</v>
@@ -6028,11 +6110,14 @@
       <c r="P38" s="11">
         <v>0</v>
       </c>
-      <c r="R38">
+      <c r="Q38" s="11">
+        <v>0</v>
+      </c>
+      <c r="S38">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D39" t="str">
         <f ca="1"/>
         <v>31-Jan</v>
@@ -6073,11 +6158,14 @@
       <c r="P39" s="11">
         <v>0</v>
       </c>
-      <c r="R39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q39" s="11">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D40" t="str">
         <f ca="1"/>
         <v>01-Feb</v>
@@ -6118,11 +6206,14 @@
       <c r="P40" s="11">
         <v>0</v>
       </c>
-      <c r="R40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q40" s="11">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D41" t="str">
         <f ca="1"/>
         <v>02-Feb</v>
@@ -6163,11 +6254,14 @@
       <c r="P41" s="11">
         <v>0</v>
       </c>
-      <c r="R41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q41" s="11">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D42" t="str">
         <f ca="1"/>
         <v>03-Feb</v>
@@ -6208,11 +6302,14 @@
       <c r="P42" s="11">
         <v>0</v>
       </c>
-      <c r="R42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q42" s="11">
+        <v>0</v>
+      </c>
+      <c r="S42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D43" t="str">
         <f ca="1"/>
         <v>04-Feb</v>
@@ -6253,11 +6350,14 @@
       <c r="P43" s="11">
         <v>0</v>
       </c>
-      <c r="R43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q43" s="11">
+        <v>0</v>
+      </c>
+      <c r="S43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D44" t="str">
         <f ca="1"/>
         <v>05-Feb</v>
@@ -6298,11 +6398,14 @@
       <c r="P44" s="11">
         <v>0</v>
       </c>
-      <c r="R44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q44" s="11">
+        <v>0</v>
+      </c>
+      <c r="S44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D45" t="str">
         <f ca="1"/>
         <v>06-Feb</v>
@@ -6343,11 +6446,14 @@
       <c r="P45" s="11">
         <v>0</v>
       </c>
-      <c r="R45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q45" s="11">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D46" t="str">
         <f ca="1"/>
         <v>07-Feb</v>
@@ -6388,11 +6494,14 @@
       <c r="P46" s="11">
         <v>0</v>
       </c>
-      <c r="R46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q46" s="11">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D47" t="str">
         <f ca="1"/>
         <v>08-Feb</v>
@@ -6433,11 +6542,14 @@
       <c r="P47" s="11">
         <v>0</v>
       </c>
-      <c r="R47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q47" s="11">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D48" t="str">
         <f ca="1"/>
         <v>09-Feb</v>
@@ -6478,11 +6590,14 @@
       <c r="P48" s="11">
         <v>0</v>
       </c>
-      <c r="R48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q48" s="11">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D49" t="str">
         <f ca="1"/>
         <v>10-Feb</v>
@@ -6523,11 +6638,14 @@
       <c r="P49" s="11">
         <v>0</v>
       </c>
-      <c r="R49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q49" s="11">
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D50" t="str">
         <f ca="1"/>
         <v>11-Feb</v>
@@ -6568,11 +6686,14 @@
       <c r="P50" s="11">
         <v>0</v>
       </c>
-      <c r="R50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q50" s="11">
+        <v>0</v>
+      </c>
+      <c r="S50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D51" t="str">
         <f ca="1"/>
         <v>12-Feb</v>
@@ -6613,11 +6734,14 @@
       <c r="P51" s="11">
         <v>0</v>
       </c>
-      <c r="R51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q51" s="11">
+        <v>0</v>
+      </c>
+      <c r="S51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D52" t="str">
         <f ca="1"/>
         <v>13-Feb</v>
@@ -6658,11 +6782,14 @@
       <c r="P52" s="11">
         <v>0</v>
       </c>
-      <c r="R52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q52" s="11">
+        <v>0</v>
+      </c>
+      <c r="S52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D53" t="str">
         <f ca="1"/>
         <v>14-Feb</v>
@@ -6703,11 +6830,14 @@
       <c r="P53" s="11">
         <v>0</v>
       </c>
-      <c r="R53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q53" s="11">
+        <v>0</v>
+      </c>
+      <c r="S53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D54" t="str">
         <f ca="1"/>
         <v>15-Feb</v>
@@ -6748,11 +6878,14 @@
       <c r="P54" s="11">
         <v>0</v>
       </c>
-      <c r="R54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q54" s="11">
+        <v>0</v>
+      </c>
+      <c r="S54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D55" t="str">
         <f ca="1"/>
         <v>16-Feb</v>
@@ -6793,11 +6926,14 @@
       <c r="P55" s="11">
         <v>0</v>
       </c>
-      <c r="R55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q55" s="11">
+        <v>0</v>
+      </c>
+      <c r="S55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D56" t="str">
         <f ca="1"/>
         <v>17-Feb</v>
@@ -6838,11 +6974,14 @@
       <c r="P56" s="11">
         <v>0</v>
       </c>
-      <c r="R56">
+      <c r="Q56" s="11">
+        <v>0</v>
+      </c>
+      <c r="S56">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D57" t="str">
         <f ca="1"/>
         <v>18-Feb</v>
@@ -6883,11 +7022,14 @@
       <c r="P57" s="11">
         <v>0</v>
       </c>
-      <c r="R57">
+      <c r="Q57" s="11">
+        <v>0</v>
+      </c>
+      <c r="S57">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D58" t="str">
         <f ca="1"/>
         <v>19-Feb</v>
@@ -6928,11 +7070,14 @@
       <c r="P58" s="11">
         <v>0</v>
       </c>
-      <c r="R58">
+      <c r="Q58" s="11">
+        <v>0</v>
+      </c>
+      <c r="S58">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D59" t="str">
         <f ca="1"/>
         <v>20-Feb</v>
@@ -6973,11 +7118,14 @@
       <c r="P59" s="11">
         <v>0</v>
       </c>
-      <c r="R59">
+      <c r="Q59" s="11">
+        <v>0</v>
+      </c>
+      <c r="S59">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D60" t="str">
         <f ca="1"/>
         <v>21-Feb</v>
@@ -7018,11 +7166,14 @@
       <c r="P60" s="11">
         <v>0</v>
       </c>
-      <c r="R60">
+      <c r="Q60" s="11">
+        <v>0</v>
+      </c>
+      <c r="S60">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D61" t="str">
         <f ca="1"/>
         <v>22-Feb</v>
@@ -7063,11 +7214,14 @@
       <c r="P61" s="11">
         <v>0</v>
       </c>
-      <c r="R61">
+      <c r="Q61" s="11">
+        <v>0</v>
+      </c>
+      <c r="S61">
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D62" t="str">
         <f ca="1"/>
         <v>23-Feb</v>
@@ -7108,11 +7262,14 @@
       <c r="P62" s="11">
         <v>0</v>
       </c>
-      <c r="R62">
+      <c r="Q62" s="11">
+        <v>0</v>
+      </c>
+      <c r="S62">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D63" t="str">
         <f ca="1"/>
         <v>24-Feb</v>
@@ -7153,11 +7310,14 @@
       <c r="P63" s="11">
         <v>0</v>
       </c>
-      <c r="R63">
+      <c r="Q63" s="11">
+        <v>0</v>
+      </c>
+      <c r="S63">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D64" t="str">
         <f ca="1"/>
         <v>25-Feb</v>
@@ -7198,11 +7358,14 @@
       <c r="P64" s="11">
         <v>0</v>
       </c>
-      <c r="R64">
+      <c r="Q64" s="11">
+        <v>0</v>
+      </c>
+      <c r="S64">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D65" t="str">
         <f ca="1"/>
         <v>26-Feb</v>
@@ -7243,11 +7406,14 @@
       <c r="P65" s="11">
         <v>0</v>
       </c>
-      <c r="R65">
+      <c r="Q65" s="11">
+        <v>0</v>
+      </c>
+      <c r="S65">
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D66" t="str">
         <f ca="1"/>
         <v>27-Feb</v>
@@ -7288,11 +7454,14 @@
       <c r="P66" s="11">
         <v>0</v>
       </c>
-      <c r="R66">
+      <c r="Q66" s="11">
+        <v>0</v>
+      </c>
+      <c r="S66">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D67" t="str">
         <f ca="1"/>
         <v>28-Feb</v>
@@ -7333,11 +7502,14 @@
       <c r="P67" s="11">
         <v>0</v>
       </c>
-      <c r="R67">
+      <c r="Q67" s="11">
+        <v>0</v>
+      </c>
+      <c r="S67">
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D68" t="str">
         <f ca="1"/>
         <v>01-Mar</v>
@@ -7378,11 +7550,14 @@
       <c r="P68" s="11">
         <v>0</v>
       </c>
-      <c r="R68">
+      <c r="Q68" s="11">
+        <v>0</v>
+      </c>
+      <c r="S68">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D69" t="str">
         <f ca="1"/>
         <v>02-Mar</v>
@@ -7423,11 +7598,14 @@
       <c r="P69" s="11">
         <v>0</v>
       </c>
-      <c r="R69">
+      <c r="Q69" s="11">
+        <v>0</v>
+      </c>
+      <c r="S69">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D70" t="str">
         <f ca="1"/>
         <v>03-Mar</v>
@@ -7468,11 +7646,14 @@
       <c r="P70" s="11">
         <v>0</v>
       </c>
-      <c r="R70">
+      <c r="Q70" s="11">
+        <v>0</v>
+      </c>
+      <c r="S70">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D71" t="str">
         <f ca="1"/>
         <v>04-Mar</v>
@@ -7513,11 +7694,14 @@
       <c r="P71" s="11">
         <v>0</v>
       </c>
-      <c r="R71">
+      <c r="Q71" s="11">
+        <v>0</v>
+      </c>
+      <c r="S71">
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D72" t="str">
         <f ca="1"/>
         <v>05-Mar</v>
@@ -7558,11 +7742,14 @@
       <c r="P72" s="11">
         <v>0</v>
       </c>
-      <c r="R72">
+      <c r="Q72" s="11">
+        <v>0</v>
+      </c>
+      <c r="S72">
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D73" t="str">
         <f ca="1"/>
         <v>06-Mar</v>
@@ -7603,11 +7790,14 @@
       <c r="P73" s="11">
         <v>0</v>
       </c>
-      <c r="R73">
+      <c r="Q73" s="11">
+        <v>0</v>
+      </c>
+      <c r="S73">
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D74" t="str">
         <f ca="1"/>
         <v>07-Mar</v>
@@ -7648,11 +7838,14 @@
       <c r="P74" s="11">
         <v>0</v>
       </c>
-      <c r="R74">
+      <c r="Q74" s="11">
+        <v>0</v>
+      </c>
+      <c r="S74">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D75" t="str">
         <f ca="1"/>
         <v>08-Mar</v>
@@ -7688,16 +7881,19 @@
         <v>0</v>
       </c>
       <c r="O75" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P75" s="11">
         <v>0</v>
       </c>
-      <c r="R75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q75" s="11">
+        <v>0</v>
+      </c>
+      <c r="S75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D76" t="str">
         <f ca="1"/>
         <v>09-Mar</v>
@@ -7733,16 +7929,19 @@
         <v>0</v>
       </c>
       <c r="O76" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P76" s="11">
         <v>0</v>
       </c>
-      <c r="R76">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="Q76" s="11">
+        <v>0</v>
+      </c>
+      <c r="S76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D77" t="str">
         <f ca="1"/>
         <v>10-Mar</v>
@@ -7778,63 +7977,69 @@
         <v>0</v>
       </c>
       <c r="O77" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P77" s="11">
-        <v>1</v>
-      </c>
-      <c r="R77">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="11">
+        <v>1</v>
+      </c>
+      <c r="S77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="D78" t="str">
+        <f ca="1"/>
+        <v>11-Mar</v>
+      </c>
+      <c r="E78" s="11">
+        <v>0</v>
+      </c>
+      <c r="F78" s="11">
+        <v>0</v>
+      </c>
+      <c r="G78" s="11">
+        <v>0</v>
+      </c>
+      <c r="H78" s="11">
+        <v>0</v>
+      </c>
+      <c r="I78" s="11">
+        <v>1</v>
+      </c>
+      <c r="J78" s="11">
+        <v>0</v>
+      </c>
+      <c r="K78" s="11">
+        <v>0</v>
+      </c>
+      <c r="L78" s="11">
+        <v>1</v>
+      </c>
+      <c r="M78" s="11">
+        <v>0</v>
+      </c>
+      <c r="N78" s="11">
+        <v>0</v>
+      </c>
+      <c r="O78" s="11">
+        <v>1</v>
+      </c>
+      <c r="P78" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q78" s="11">
+        <v>0</v>
+      </c>
+      <c r="S78">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D78" t="str">
-        <f ca="1"/>
-        <v>11-Mar</v>
-      </c>
-      <c r="E78" s="11">
-        <v>0</v>
-      </c>
-      <c r="F78" s="11">
-        <v>0</v>
-      </c>
-      <c r="G78" s="11">
-        <v>0</v>
-      </c>
-      <c r="H78" s="11">
-        <v>0</v>
-      </c>
-      <c r="I78" s="11">
-        <v>1</v>
-      </c>
-      <c r="J78" s="11">
-        <v>0</v>
-      </c>
-      <c r="K78" s="11">
-        <v>0</v>
-      </c>
-      <c r="L78" s="11">
-        <v>1</v>
-      </c>
-      <c r="M78" s="11">
-        <v>0</v>
-      </c>
-      <c r="N78" s="11">
-        <v>0</v>
-      </c>
-      <c r="O78" s="11">
-        <v>0</v>
-      </c>
-      <c r="P78" s="11">
-        <v>0</v>
-      </c>
-      <c r="R78">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="D9:P78">
-    <cfRule type="expression" dxfId="7" priority="1">
+  <conditionalFormatting sqref="D9:Q78">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(D9)-ROW($D$8),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
So far for today
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC26EC8D-E592-4634-B179-520A869B785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97874637-8369-42E9-9B2F-777B70A5FBA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -32,7 +32,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">_xlfn.DROP(_xlfn._TRO_ALL(Report!$B:$K),1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -601,28 +600,7 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <fill>
         <patternFill>
@@ -883,27 +861,27 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Standard Pivot Table" table="0" count="12" xr9:uid="{94886349-6B4A-4300-89B0-9F83C8B5183A}">
-      <tableStyleElement type="wholeTable" dxfId="25"/>
-      <tableStyleElement type="headerRow" dxfId="24"/>
-      <tableStyleElement type="totalRow" dxfId="23"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="22"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="21"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="20"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="19"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="18"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="17"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="16"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="15"/>
-      <tableStyleElement type="pageFieldValues" dxfId="14"/>
+      <tableStyleElement type="wholeTable" dxfId="22"/>
+      <tableStyleElement type="headerRow" dxfId="21"/>
+      <tableStyleElement type="totalRow" dxfId="20"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="19"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="18"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="17"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="16"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="14"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="13"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="12"/>
+      <tableStyleElement type="pageFieldValues" dxfId="11"/>
     </tableStyle>
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="13"/>
-      <tableStyleElement type="headerRow" dxfId="12"/>
-      <tableStyleElement type="totalRow" dxfId="11"/>
-      <tableStyleElement type="firstColumn" dxfId="10"/>
-      <tableStyleElement type="lastColumn" dxfId="9"/>
-      <tableStyleElement type="firstRowStripe" dxfId="8"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="7"/>
+      <tableStyleElement type="wholeTable" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="totalRow" dxfId="8"/>
+      <tableStyleElement type="firstColumn" dxfId="7"/>
+      <tableStyleElement type="lastColumn" dxfId="6"/>
+      <tableStyleElement type="firstRowStripe" dxfId="5"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -956,7 +934,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$O$9:$X$18" spid="_x0000_s2292"/>
+                  <a14:cameraTool cellRange="$O$9:$X$18" spid="_x0000_s2299"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1310,7 +1288,7 @@
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="O82" sqref="O82"/>
+      <selection pane="bottomLeft" activeCell="V81" sqref="V81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1399,7 +1377,7 @@
     </row>
     <row r="10" spans="1:27" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="str" cm="1">
-        <f t="array" aca="1" ref="B10:B81" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
+        <f t="array" aca="1" ref="B10:B82" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
         <v>01-Jan</v>
       </c>
       <c r="C10" s="5"/>
@@ -1412,7 +1390,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="12"/>
       <c r="M10" cm="1">
-        <f t="array" ref="M10:M81">_xlfn.BYROW(_xlfn.DROP(Banded,,1),_xleta.SUM)</f>
+        <f t="array" ref="M10:M82">_xlfn.BYROW(_xlfn.DROP(Banded,,1),_xleta.SUM)</f>
         <v>0</v>
       </c>
       <c r="O10" s="14" cm="1">
@@ -1893,39 +1871,39 @@
       </c>
       <c r="P18" s="11">
         <f ca="1"/>
+        <v>6</v>
+      </c>
+      <c r="Q18" s="11">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="R18" s="11">
+        <f ca="1"/>
         <v>5</v>
       </c>
-      <c r="Q18" s="11">
-        <f ca="1"/>
-        <v>4</v>
-      </c>
-      <c r="R18" s="11">
+      <c r="S18" s="11">
+        <f ca="1"/>
+        <v>6</v>
+      </c>
+      <c r="T18" s="11">
+        <f ca="1"/>
+        <v>6</v>
+      </c>
+      <c r="U18" s="11">
         <f ca="1"/>
         <v>5</v>
       </c>
-      <c r="S18" s="11">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="T18" s="11">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="U18" s="11">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
       <c r="V18" s="11">
         <f ca="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W18" s="11">
         <f ca="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X18" s="11">
         <f ca="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="2:24" x14ac:dyDescent="0.25">
@@ -1998,7 +1976,7 @@
         <v>0</v>
       </c>
       <c r="L21" cm="1">
-        <f t="array" aca="1" ref="L21:L81" ca="1">WEEKNUM(_date+0)</f>
+        <f t="array" aca="1" ref="L21:L82" ca="1">WEEKNUM(_date+0)</f>
         <v>3</v>
       </c>
       <c r="M21">
@@ -4410,16 +4388,44 @@
       </c>
     </row>
     <row r="82" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B82" s="9"/>
-      <c r="C82" s="16"/>
-      <c r="D82" s="16"/>
-      <c r="E82" s="16"/>
-      <c r="F82" s="16"/>
-      <c r="G82" s="16"/>
-      <c r="H82" s="16"/>
-      <c r="I82" s="16"/>
-      <c r="J82" s="16"/>
-      <c r="K82" s="16"/>
+      <c r="B82" s="9" t="str">
+        <f ca="1"/>
+        <v>14-Mar</v>
+      </c>
+      <c r="C82" s="16">
+        <v>1</v>
+      </c>
+      <c r="D82" s="16">
+        <v>0</v>
+      </c>
+      <c r="E82" s="16">
+        <v>0</v>
+      </c>
+      <c r="F82" s="16">
+        <v>1</v>
+      </c>
+      <c r="G82" s="16">
+        <v>1</v>
+      </c>
+      <c r="H82" s="16">
+        <v>0</v>
+      </c>
+      <c r="I82" s="16">
+        <v>1</v>
+      </c>
+      <c r="J82" s="16">
+        <v>1</v>
+      </c>
+      <c r="K82" s="16">
+        <v>1</v>
+      </c>
+      <c r="L82">
+        <f ca="1"/>
+        <v>11</v>
+      </c>
+      <c r="M82">
+        <v>6</v>
+      </c>
     </row>
     <row r="83" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B83" s="9"/>
@@ -4630,17 +4636,17 @@
     <sortCondition ref="Q24:Q60"/>
   </sortState>
   <conditionalFormatting sqref="B10:K81">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>MOD(ROW(XEJ10)-ROW($O$9),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:K77">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>MOD(ROW(XEM10)-ROW($O$9),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9:X18">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>MOD(ROW(O9)-ROW($O$9),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4692,12 +4698,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7275F8F4-F02E-491D-8929-12439DC1AD26}">
-  <dimension ref="D7:S80"/>
+  <dimension ref="D7:S81"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="E80" sqref="E80:Q80"/>
+      <selection pane="bottomLeft" activeCell="Q81" sqref="Q81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4707,7 +4713,7 @@
   </cols>
   <sheetData>
     <row r="7" spans="4:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="4:19" ht="154.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:19" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>0</v>
       </c>
@@ -4753,7 +4759,7 @@
     </row>
     <row r="9" spans="4:19" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D9" t="str" cm="1">
-        <f t="array" aca="1" ref="D9:D80" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
+        <f t="array" aca="1" ref="D9:D81" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
         <v>01-Jan</v>
       </c>
       <c r="E9" s="11">
@@ -4796,7 +4802,7 @@
         <v>0</v>
       </c>
       <c r="S9" cm="1">
-        <f t="array" ref="S9:S80">_xlfn.BYROW(_xlfn.DROP(_xlnm.Print_Area,,1),_xleta.SUM)</f>
+        <f t="array" ref="S9:S81">_xlfn.BYROW(_xlfn.DROP(_xlnm.Print_Area,,1),_xleta.SUM)</f>
         <v>0</v>
       </c>
     </row>
@@ -8196,7 +8202,7 @@
         <v>0</v>
       </c>
       <c r="O80" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P80" s="11">
         <v>0</v>
@@ -8205,12 +8211,60 @@
         <v>1</v>
       </c>
       <c r="S80">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="D81" t="str">
+        <f ca="1"/>
+        <v>14-Mar</v>
+      </c>
+      <c r="E81" s="11">
+        <v>0</v>
+      </c>
+      <c r="F81" s="11">
+        <v>0</v>
+      </c>
+      <c r="G81" s="11">
+        <v>0</v>
+      </c>
+      <c r="H81" s="11">
+        <v>0</v>
+      </c>
+      <c r="I81" s="11">
+        <v>1</v>
+      </c>
+      <c r="J81" s="11">
+        <v>0</v>
+      </c>
+      <c r="K81" s="11">
+        <v>0</v>
+      </c>
+      <c r="L81" s="11">
+        <v>1</v>
+      </c>
+      <c r="M81" s="11">
+        <v>0</v>
+      </c>
+      <c r="N81" s="11">
+        <v>0</v>
+      </c>
+      <c r="O81" s="11">
+        <v>0</v>
+      </c>
+      <c r="P81" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q81" s="11">
+        <v>1</v>
+      </c>
+      <c r="S81">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D9:Q79">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(D9)-ROW($D$8),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Finishing up at the cabin
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{037874D4-C90A-4993-B8AA-3B0EEADF59EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09143AF5-787C-4B28-BE00-A9E84C601C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">_xlfn.DROP(_xlfn._TRO_ALL(Report!$B:$K),1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -945,7 +944,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$O$9:$X$19" spid="_x0000_s2339"/>
+                  <a14:cameraTool cellRange="$O$9:$X$19" spid="_x0000_s2344"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1299,7 +1298,7 @@
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A9" sqref="A9"/>
-      <selection pane="bottomLeft" activeCell="O88" sqref="O87:O88"/>
+      <selection pane="bottomLeft" activeCell="O91" sqref="O91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1391,7 +1390,7 @@
     </row>
     <row r="10" spans="1:27" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="str" cm="1">
-        <f t="array" aca="1" ref="B10:B85" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
+        <f t="array" aca="1" ref="B10:B86" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
         <v>01-Jan</v>
       </c>
       <c r="C10" s="5"/>
@@ -1404,7 +1403,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="12"/>
       <c r="M10" cm="1">
-        <f t="array" ref="M10:M85">_xlfn.BYROW(_xlfn.DROP(Banded,,1),_xleta.SUM)</f>
+        <f t="array" ref="M10:M86">_xlfn.BYROW(_xlfn.DROP(Banded,,1),_xleta.SUM)</f>
         <v>0</v>
       </c>
       <c r="O10" s="14" cm="1">
@@ -1943,39 +1942,39 @@
       </c>
       <c r="P19" s="11">
         <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="Q19" s="11">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R19" s="11">
+        <f ca="1"/>
         <v>2</v>
       </c>
-      <c r="Q19" s="11">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="R19" s="11">
+      <c r="S19" s="11">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="T19" s="11">
         <f ca="1"/>
         <v>2</v>
       </c>
-      <c r="S19" s="11">
+      <c r="U19" s="11">
         <f ca="1"/>
         <v>2</v>
       </c>
-      <c r="T19" s="11">
+      <c r="V19" s="11">
         <f ca="1"/>
         <v>2</v>
       </c>
-      <c r="U19" s="11">
-        <f ca="1"/>
-        <v>2</v>
-      </c>
-      <c r="V19" s="11">
-        <f ca="1"/>
-        <v>2</v>
-      </c>
       <c r="W19" s="11">
         <f ca="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X19" s="11">
         <f ca="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.25">
@@ -2030,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="L21" cm="1">
-        <f t="array" aca="1" ref="L21:L85" ca="1">WEEKNUM(_date+0)</f>
+        <f t="array" aca="1" ref="L21:L86" ca="1">WEEKNUM(_date+0)</f>
         <v>3</v>
       </c>
       <c r="M21">
@@ -4602,16 +4601,44 @@
       </c>
     </row>
     <row r="86" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B86" s="9"/>
-      <c r="C86" s="16"/>
-      <c r="D86" s="16"/>
-      <c r="E86" s="16"/>
-      <c r="F86" s="16"/>
-      <c r="G86" s="16"/>
-      <c r="H86" s="16"/>
-      <c r="I86" s="16"/>
-      <c r="J86" s="16"/>
-      <c r="K86" s="16"/>
+      <c r="B86" s="9" t="str">
+        <f ca="1"/>
+        <v>18-Mar</v>
+      </c>
+      <c r="C86" s="16">
+        <v>1</v>
+      </c>
+      <c r="D86" s="16">
+        <v>0</v>
+      </c>
+      <c r="E86" s="16">
+        <v>0</v>
+      </c>
+      <c r="F86" s="16">
+        <v>1</v>
+      </c>
+      <c r="G86" s="16">
+        <v>0</v>
+      </c>
+      <c r="H86" s="16">
+        <v>0</v>
+      </c>
+      <c r="I86" s="16">
+        <v>0</v>
+      </c>
+      <c r="J86" s="16">
+        <v>1</v>
+      </c>
+      <c r="K86" s="16">
+        <v>1</v>
+      </c>
+      <c r="L86">
+        <f ca="1"/>
+        <v>12</v>
+      </c>
+      <c r="M86">
+        <v>4</v>
+      </c>
     </row>
     <row r="87" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B87" s="9"/>
@@ -4836,12 +4863,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7275F8F4-F02E-491D-8929-12439DC1AD26}">
-  <dimension ref="D7:S84"/>
+  <dimension ref="D7:S85"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="S89" sqref="S89"/>
+      <selection pane="bottomLeft" activeCell="V95" sqref="V95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4851,7 +4878,7 @@
   </cols>
   <sheetData>
     <row r="7" spans="4:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="4:19" ht="132" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:19" ht="131.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>0</v>
       </c>
@@ -4897,7 +4924,7 @@
     </row>
     <row r="9" spans="4:19" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D9" t="str" cm="1">
-        <f t="array" aca="1" ref="D9:D84" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
+        <f t="array" aca="1" ref="D9:D85" ca="1">TEXT(DATE(2025,1,_xlfn.SEQUENCE(1+_xlfn.DAYS(TODAY(),DATE(2025,1,1)))),"dd-mmm")</f>
         <v>01-Jan</v>
       </c>
       <c r="E9" s="11">
@@ -4940,7 +4967,7 @@
         <v>0</v>
       </c>
       <c r="S9" cm="1">
-        <f t="array" ref="S9:S84">_xlfn.BYROW(_xlfn.DROP(_xlnm.Print_Area,,1),_xleta.SUM)</f>
+        <f t="array" ref="S9:S85">_xlfn.BYROW(_xlfn.DROP(_xlnm.Print_Area,,1),_xleta.SUM)</f>
         <v>0</v>
       </c>
     </row>
@@ -8542,6 +8569,54 @@
       </c>
       <c r="S84">
         <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="D85" t="str">
+        <f ca="1"/>
+        <v>18-Mar</v>
+      </c>
+      <c r="E85" s="11">
+        <v>0</v>
+      </c>
+      <c r="F85" s="11">
+        <v>0</v>
+      </c>
+      <c r="G85" s="11">
+        <v>0</v>
+      </c>
+      <c r="H85" s="11">
+        <v>0</v>
+      </c>
+      <c r="I85" s="11">
+        <v>1</v>
+      </c>
+      <c r="J85" s="11">
+        <v>0</v>
+      </c>
+      <c r="K85" s="11">
+        <v>0</v>
+      </c>
+      <c r="L85" s="11">
+        <v>1</v>
+      </c>
+      <c r="M85" s="11">
+        <v>0</v>
+      </c>
+      <c r="N85" s="11">
+        <v>0</v>
+      </c>
+      <c r="O85" s="11">
+        <v>0</v>
+      </c>
+      <c r="P85" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q85" s="11">
+        <v>1</v>
+      </c>
+      <c r="S85">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done with today's minimum
</commit_message>
<xml_diff>
--- a/DailyPlanningTemplate.xlsx
+++ b/DailyPlanningTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4E89C1-DFB8-45EA-9E37-0E4A83383779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26F2245-CDE4-40E8-A7BC-62C9E23D34A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -954,7 +954,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$O$9:$X$20" spid="_x0000_s2398"/>
+                  <a14:cameraTool cellRange="$O$9:$X$20" spid="_x0000_s2399"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1308,7 +1308,7 @@
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="N88" sqref="N88"/>
+      <selection pane="bottomLeft" activeCell="W88" sqref="W88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2030,7 +2030,7 @@
       </c>
       <c r="U20" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V20" s="11">
         <f ca="1"/>
@@ -4870,7 +4870,7 @@
         <v>1</v>
       </c>
       <c r="H91" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I91" s="16">
         <v>1</v>
@@ -4886,7 +4886,7 @@
         <v>13</v>
       </c>
       <c r="M91">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>